<commit_message>
ran model for jan 6
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Documents\NBAPredictiveModel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A37986-A548-4E1C-89AB-89248B185B02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -52,6 +58,39 @@
     <t>POR</t>
   </si>
   <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>PHI</t>
+  </si>
+  <si>
+    <t>ORL</t>
+  </si>
+  <si>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>ATL</t>
+  </si>
+  <si>
+    <t>NYK</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>MIL</t>
+  </si>
+  <si>
+    <t>PHO</t>
+  </si>
+  <si>
+    <t>SAC</t>
+  </si>
+  <si>
+    <t>GSW</t>
+  </si>
+  <si>
     <t>UTA</t>
   </si>
   <si>
@@ -65,16 +104,46 @@
   </si>
   <si>
     <t>CHI</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
+    <t>WAS</t>
+  </si>
+  <si>
+    <t>CLE</t>
+  </si>
+  <si>
+    <t>BOS</t>
+  </si>
+  <si>
+    <t>CHO</t>
+  </si>
+  <si>
+    <t>OKC</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>TOR</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +207,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -184,7 +261,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -216,9 +293,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,6 +345,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,14 +538,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44201</v>
       </c>
@@ -463,7 +579,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <v>-4.5</v>
@@ -474,8 +590,11 @@
       <c r="F2">
         <v>-1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44201</v>
       </c>
@@ -483,7 +602,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>9.5</v>
@@ -494,8 +613,11 @@
       <c r="F3">
         <v>-6.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44201</v>
       </c>
@@ -503,7 +625,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D4">
         <v>-10.5</v>
@@ -514,8 +636,11 @@
       <c r="F4">
         <v>-1.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44201</v>
       </c>
@@ -523,19 +648,22 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D5">
         <v>-9.5</v>
       </c>
       <c r="E5">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F5">
         <v>-11.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44201</v>
       </c>
@@ -543,7 +671,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D6">
         <v>-9.5</v>
@@ -552,7 +680,230 @@
         <v>7.4</v>
       </c>
       <c r="F6">
-        <v>-16.9</v>
+        <v>-16.899999999999999</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>-2.5</v>
+      </c>
+      <c r="E7">
+        <v>-3</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8">
+        <v>-6.5</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+      <c r="F8">
+        <v>-6.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>-6</v>
+      </c>
+      <c r="E9">
+        <v>-6.2</v>
+      </c>
+      <c r="F9">
+        <v>0.20000000000000021</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10">
+        <v>-2.5</v>
+      </c>
+      <c r="E10">
+        <v>0.8</v>
+      </c>
+      <c r="F10">
+        <v>-3.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>-6</v>
+      </c>
+      <c r="E11">
+        <v>-7.8</v>
+      </c>
+      <c r="F11">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>7.5</v>
+      </c>
+      <c r="E12">
+        <v>6.3</v>
+      </c>
+      <c r="F12">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13">
+        <v>-8</v>
+      </c>
+      <c r="E13">
+        <v>2.9</v>
+      </c>
+      <c r="F13">
+        <v>-10.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14">
+        <v>-12</v>
+      </c>
+      <c r="E14">
+        <v>-22.6</v>
+      </c>
+      <c r="F14">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15">
+        <v>-3</v>
+      </c>
+      <c r="E15">
+        <v>-10.4</v>
+      </c>
+      <c r="F15">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16">
+        <v>-7</v>
+      </c>
+      <c r="E16">
+        <v>7.2</v>
+      </c>
+      <c r="F16">
+        <v>-14.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>-1</v>
+      </c>
+      <c r="E17">
+        <v>-3.5</v>
+      </c>
+      <c r="F17">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran model for jan 7
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A37986-A548-4E1C-89AB-89248B185B02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78D8CBD-307F-4202-A590-876F227ECDA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -91,12 +91,12 @@
     <t>GSW</t>
   </si>
   <si>
+    <t>LAL</t>
+  </si>
+  <si>
     <t>UTA</t>
   </si>
   <si>
-    <t>LAL</t>
-  </si>
-  <si>
     <t>MIN</t>
   </si>
   <si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>TOR</t>
+  </si>
+  <si>
+    <t>DAL</t>
   </si>
   <si>
     <t>No</t>
@@ -539,13 +542,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -579,7 +589,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <v>-4.5</v>
@@ -591,7 +601,7 @@
         <v>-1</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -602,7 +612,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3">
         <v>9.5</v>
@@ -614,7 +624,7 @@
         <v>-6.1</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -637,7 +647,7 @@
         <v>-1.6</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -660,7 +670,7 @@
         <v>-11.8</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -683,7 +693,7 @@
         <v>-16.899999999999999</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -705,6 +715,9 @@
       <c r="F7">
         <v>0.5</v>
       </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -725,6 +738,9 @@
       <c r="F8">
         <v>-6.6</v>
       </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -745,6 +761,9 @@
       <c r="F9">
         <v>0.20000000000000021</v>
       </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
@@ -765,6 +784,9 @@
       <c r="F10">
         <v>-3.3</v>
       </c>
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
@@ -785,6 +807,9 @@
       <c r="F11">
         <v>1.8</v>
       </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
@@ -794,7 +819,7 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D12">
         <v>7.5</v>
@@ -804,6 +829,9 @@
       </c>
       <c r="F12">
         <v>1.2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -825,6 +853,9 @@
       <c r="F13">
         <v>-10.9</v>
       </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
@@ -845,6 +876,9 @@
       <c r="F14">
         <v>10.6</v>
       </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
@@ -865,6 +899,9 @@
       <c r="F15">
         <v>7.4</v>
       </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
@@ -885,8 +922,11 @@
       <c r="F16">
         <v>-14.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44202</v>
       </c>
@@ -897,13 +937,116 @@
         <v>10</v>
       </c>
       <c r="D17">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="E17">
         <v>-3.5</v>
       </c>
       <c r="F17">
-        <v>2.5</v>
+        <v>8.5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18">
+        <v>1.5</v>
+      </c>
+      <c r="E18">
+        <v>2.6</v>
+      </c>
+      <c r="F18">
+        <v>-1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <v>-5</v>
+      </c>
+      <c r="E19">
+        <v>-7.9</v>
+      </c>
+      <c r="F19">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>-10</v>
+      </c>
+      <c r="E20">
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="F20">
+        <v>-5.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>-2.5</v>
+      </c>
+      <c r="E21">
+        <v>-11.4</v>
+      </c>
+      <c r="F21">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22">
+        <v>-7</v>
+      </c>
+      <c r="E22">
+        <v>-6.1</v>
+      </c>
+      <c r="F22">
+        <v>-0.90000000000000036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Excel sheet to show success rate
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -5,22 +5,32 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Documents\NBAPredictiveModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78D8CBD-307F-4202-A590-876F227ECDA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79E9413-C23C-4484-8F90-26E75A5943A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -137,6 +147,15 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Total Wins</t>
+  </si>
+  <si>
+    <t>Total Played</t>
+  </si>
+  <si>
+    <t>Success Rate</t>
   </si>
 </sst>
 </file>
@@ -146,7 +165,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +175,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -195,18 +221,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -542,23 +571,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44201</v>
       </c>
@@ -603,8 +628,15 @@
       <c r="G2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2">
+        <f>COUNTIF(G:G, "Yes")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44201</v>
       </c>
@@ -626,8 +658,15 @@
       <c r="G3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3">
+        <f>COUNTIF(G:G, "*")</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44201</v>
       </c>
@@ -649,8 +688,15 @@
       <c r="G4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="3">
+        <f>IF(J3=0, 0, J2/J3)</f>
+        <v>0.70588235294117652</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44201</v>
       </c>
@@ -673,7 +719,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44201</v>
       </c>
@@ -696,7 +742,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>44202</v>
       </c>
@@ -719,7 +765,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>44202</v>
       </c>
@@ -742,7 +788,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>44202</v>
       </c>
@@ -765,7 +811,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>44202</v>
       </c>
@@ -788,7 +834,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44202</v>
       </c>
@@ -811,7 +857,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>44202</v>
       </c>
@@ -834,7 +880,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44202</v>
       </c>
@@ -857,7 +903,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>44202</v>
       </c>
@@ -880,7 +926,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>44202</v>
       </c>
@@ -903,7 +949,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>44202</v>
       </c>
@@ -963,10 +1009,10 @@
         <v>1.5</v>
       </c>
       <c r="E18">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="F18">
-        <v>-1.1000000000000001</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -983,10 +1029,10 @@
         <v>-5</v>
       </c>
       <c r="E19">
-        <v>-7.9</v>
+        <v>-7.8</v>
       </c>
       <c r="F19">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1023,10 +1069,10 @@
         <v>-2.5</v>
       </c>
       <c r="E21">
-        <v>-11.4</v>
+        <v>-11.5</v>
       </c>
       <c r="F21">
-        <v>8.9</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1043,10 +1089,10 @@
         <v>-7</v>
       </c>
       <c r="E22">
-        <v>-6.1</v>
+        <v>-6.2</v>
       </c>
       <c r="F22">
-        <v>-0.90000000000000036</v>
+        <v>-0.79999999999999982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran model for jan 8
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -5,32 +5,22 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79E9413-C23C-4484-8F90-26E75A5943A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C048BC8-24A4-4B5D-97A3-D8D41CE735AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3084" yWindow="1260" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -53,6 +43,15 @@
     <t>Beat Vegas?</t>
   </si>
   <si>
+    <t>Unnamed: 7</t>
+  </si>
+  <si>
+    <t>Unnamed: 8</t>
+  </si>
+  <si>
+    <t>Unnamed: 9</t>
+  </si>
+  <si>
     <t>BRK</t>
   </si>
   <si>
@@ -104,6 +103,15 @@
     <t>LAL</t>
   </si>
   <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>BOS</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
     <t>UTA</t>
   </si>
   <si>
@@ -116,25 +124,16 @@
     <t>CHI</t>
   </si>
   <si>
-    <t>HOU</t>
-  </si>
-  <si>
     <t>WAS</t>
   </si>
   <si>
     <t>CLE</t>
   </si>
   <si>
-    <t>BOS</t>
-  </si>
-  <si>
     <t>CHO</t>
   </si>
   <si>
     <t>OKC</t>
-  </si>
-  <si>
-    <t>DET</t>
   </si>
   <si>
     <t>TOR</t>
@@ -165,7 +164,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,13 +174,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -221,21 +213,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -571,16 +560,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -605,16 +591,25 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44201</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>-4.5</v>
@@ -626,14 +621,13 @@
         <v>-1</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J2">
-        <f>COUNTIF(G:G, "Yes")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -641,10 +635,10 @@
         <v>44201</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>9.5</v>
@@ -656,14 +650,13 @@
         <v>-6.1</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J3">
-        <f>COUNTIF(G:G, "*")</f>
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -671,10 +664,10 @@
         <v>44201</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D4">
         <v>-10.5</v>
@@ -686,14 +679,13 @@
         <v>-1.6</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="3">
-        <f>IF(J3=0, 0, J2/J3)</f>
-        <v>0.70588235294117652</v>
+        <v>44</v>
+      </c>
+      <c r="J4">
+        <v>0.59090909090909094</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -701,10 +693,10 @@
         <v>44201</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>-9.5</v>
@@ -716,7 +708,7 @@
         <v>-11.8</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -724,10 +716,10 @@
         <v>44201</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <v>-9.5</v>
@@ -739,7 +731,7 @@
         <v>-16.899999999999999</v>
       </c>
       <c r="G6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -747,10 +739,10 @@
         <v>44202</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>-2.5</v>
@@ -762,7 +754,7 @@
         <v>0.5</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -770,10 +762,10 @@
         <v>44202</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D8">
         <v>-6.5</v>
@@ -785,7 +777,7 @@
         <v>-6.6</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -793,10 +785,10 @@
         <v>44202</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>-6</v>
@@ -808,7 +800,7 @@
         <v>0.20000000000000021</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -816,10 +808,10 @@
         <v>44202</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10">
         <v>-2.5</v>
@@ -831,7 +823,7 @@
         <v>-3.3</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -839,10 +831,10 @@
         <v>44202</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D11">
         <v>-6</v>
@@ -854,7 +846,7 @@
         <v>1.8</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -862,10 +854,10 @@
         <v>44202</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D12">
         <v>7.5</v>
@@ -877,7 +869,7 @@
         <v>1.2</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -885,10 +877,10 @@
         <v>44202</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D13">
         <v>-8</v>
@@ -900,7 +892,7 @@
         <v>-10.9</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -908,10 +900,10 @@
         <v>44202</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D14">
         <v>-12</v>
@@ -923,7 +915,7 @@
         <v>10.6</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -931,10 +923,10 @@
         <v>44202</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D15">
         <v>-3</v>
@@ -946,7 +938,7 @@
         <v>7.4</v>
       </c>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -954,10 +946,10 @@
         <v>44202</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D16">
         <v>-7</v>
@@ -969,7 +961,7 @@
         <v>-14.2</v>
       </c>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -977,10 +969,10 @@
         <v>44202</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -992,7 +984,7 @@
         <v>8.5</v>
       </c>
       <c r="G17" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1000,10 +992,10 @@
         <v>44203</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>1.5</v>
@@ -1013,6 +1005,9 @@
       </c>
       <c r="F18">
         <v>-1.2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1020,10 +1015,10 @@
         <v>44203</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D19">
         <v>-5</v>
@@ -1033,6 +1028,9 @@
       </c>
       <c r="F19">
         <v>2.8</v>
+      </c>
+      <c r="G19" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1040,10 +1038,10 @@
         <v>44203</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D20">
         <v>-10</v>
@@ -1053,6 +1051,9 @@
       </c>
       <c r="F20">
         <v>-5.6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1060,10 +1061,10 @@
         <v>44203</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D21">
         <v>-2.5</v>
@@ -1073,6 +1074,9 @@
       </c>
       <c r="F21">
         <v>9</v>
+      </c>
+      <c r="G21" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1080,10 +1084,10 @@
         <v>44203</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D22">
         <v>-7</v>
@@ -1093,6 +1097,209 @@
       </c>
       <c r="F22">
         <v>-0.79999999999999982</v>
+      </c>
+      <c r="G22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>9.4</v>
+      </c>
+      <c r="F23">
+        <v>-1.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24">
+        <v>-7</v>
+      </c>
+      <c r="E24">
+        <v>-1.6</v>
+      </c>
+      <c r="F24">
+        <v>-5.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25">
+        <v>-4.5</v>
+      </c>
+      <c r="E25">
+        <v>3.4</v>
+      </c>
+      <c r="F25">
+        <v>-7.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26">
+        <v>-2.5</v>
+      </c>
+      <c r="E26">
+        <v>2.5</v>
+      </c>
+      <c r="F26">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27">
+        <v>-5.5</v>
+      </c>
+      <c r="E27">
+        <v>-20.3</v>
+      </c>
+      <c r="F27">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28">
+        <v>-6.5</v>
+      </c>
+      <c r="E28">
+        <v>-5.2</v>
+      </c>
+      <c r="F28">
+        <v>-1.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>-1</v>
+      </c>
+      <c r="E29">
+        <v>16.7</v>
+      </c>
+      <c r="F29">
+        <v>-17.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>-6.4</v>
+      </c>
+      <c r="F30">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31">
+        <v>6.5</v>
+      </c>
+      <c r="E31">
+        <v>-3.9</v>
+      </c>
+      <c r="F31">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32">
+        <v>-9.5</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>-10.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran model for 1/09/2021
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -5,22 +5,32 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Documents\NBAPredictiveModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C048BC8-24A4-4B5D-97A3-D8D41CE735AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5614A4-AABC-433D-890D-9AD7767D5C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3084" yWindow="1260" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -43,15 +53,6 @@
     <t>Beat Vegas?</t>
   </si>
   <si>
-    <t>Unnamed: 7</t>
-  </si>
-  <si>
-    <t>Unnamed: 8</t>
-  </si>
-  <si>
-    <t>Unnamed: 9</t>
-  </si>
-  <si>
     <t>BRK</t>
   </si>
   <si>
@@ -112,49 +113,40 @@
     <t>HOU</t>
   </si>
   <si>
+    <t>WAS</t>
+  </si>
+  <si>
+    <t>CHO</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
     <t>UTA</t>
   </si>
   <si>
-    <t>MIN</t>
-  </si>
-  <si>
     <t>SAS</t>
   </si>
   <si>
     <t>CHI</t>
   </si>
   <si>
-    <t>WAS</t>
-  </si>
-  <si>
     <t>CLE</t>
   </si>
   <si>
-    <t>CHO</t>
-  </si>
-  <si>
     <t>OKC</t>
   </si>
   <si>
     <t>TOR</t>
   </si>
   <si>
-    <t>DAL</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>Total Wins</t>
-  </si>
-  <si>
-    <t>Total Played</t>
-  </si>
-  <si>
-    <t>Success Rate</t>
   </si>
 </sst>
 </file>
@@ -560,9 +552,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -591,25 +585,16 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44201</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2">
         <v>-4.5</v>
@@ -621,13 +606,7 @@
         <v>-1</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -635,10 +614,10 @@
         <v>44201</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3">
         <v>9.5</v>
@@ -650,13 +629,7 @@
         <v>-6.1</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -664,10 +637,10 @@
         <v>44201</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>-10.5</v>
@@ -679,13 +652,7 @@
         <v>-1.6</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4">
-        <v>0.59090909090909094</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -693,7 +660,7 @@
         <v>44201</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
@@ -708,7 +675,7 @@
         <v>-11.8</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -716,7 +683,7 @@
         <v>44201</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -731,7 +698,7 @@
         <v>-16.899999999999999</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -739,10 +706,10 @@
         <v>44202</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D7">
         <v>-2.5</v>
@@ -754,7 +721,11 @@
         <v>0.5</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="J7">
+        <f>COUNTIF(G2:G32, "Yes")</f>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -762,10 +733,10 @@
         <v>44202</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D8">
         <v>-6.5</v>
@@ -777,7 +748,11 @@
         <v>-6.6</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="J8">
+        <f>COUNTIF(G2:G32, "*")</f>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -785,10 +760,10 @@
         <v>44202</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9">
         <v>-6</v>
@@ -800,7 +775,11 @@
         <v>0.20000000000000021</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="J9">
+        <f>J7/J8</f>
+        <v>0.54838709677419351</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -808,10 +787,10 @@
         <v>44202</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>-2.5</v>
@@ -823,7 +802,7 @@
         <v>-3.3</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -831,10 +810,10 @@
         <v>44202</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D11">
         <v>-6</v>
@@ -846,7 +825,7 @@
         <v>1.8</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -854,10 +833,10 @@
         <v>44202</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12">
         <v>7.5</v>
@@ -869,7 +848,7 @@
         <v>1.2</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -877,10 +856,10 @@
         <v>44202</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13">
         <v>-8</v>
@@ -892,7 +871,7 @@
         <v>-10.9</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -900,10 +879,10 @@
         <v>44202</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D14">
         <v>-12</v>
@@ -915,7 +894,7 @@
         <v>10.6</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -923,10 +902,10 @@
         <v>44202</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D15">
         <v>-3</v>
@@ -938,7 +917,7 @@
         <v>7.4</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -946,7 +925,7 @@
         <v>44202</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
         <v>33</v>
@@ -961,7 +940,7 @@
         <v>-14.2</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -969,10 +948,10 @@
         <v>44202</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -984,7 +963,7 @@
         <v>8.5</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -992,10 +971,10 @@
         <v>44203</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D18">
         <v>1.5</v>
@@ -1007,7 +986,7 @@
         <v>-1.2</v>
       </c>
       <c r="G18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1015,10 +994,10 @@
         <v>44203</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19">
         <v>-5</v>
@@ -1030,7 +1009,7 @@
         <v>2.8</v>
       </c>
       <c r="G19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1038,10 +1017,10 @@
         <v>44203</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D20">
         <v>-10</v>
@@ -1053,7 +1032,7 @@
         <v>-5.6</v>
       </c>
       <c r="G20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1061,10 +1040,10 @@
         <v>44203</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D21">
         <v>-2.5</v>
@@ -1076,7 +1055,7 @@
         <v>9</v>
       </c>
       <c r="G21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1084,7 +1063,7 @@
         <v>44203</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
@@ -1099,7 +1078,7 @@
         <v>-0.79999999999999982</v>
       </c>
       <c r="G22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1107,10 +1086,10 @@
         <v>44204</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D23">
         <v>8</v>
@@ -1120,6 +1099,9 @@
       </c>
       <c r="F23">
         <v>-1.4</v>
+      </c>
+      <c r="G23" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1127,10 +1109,10 @@
         <v>44204</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D24">
         <v>-7</v>
@@ -1140,6 +1122,9 @@
       </c>
       <c r="F24">
         <v>-5.4</v>
+      </c>
+      <c r="G24" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1147,10 +1132,10 @@
         <v>44204</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D25">
         <v>-4.5</v>
@@ -1160,6 +1145,9 @@
       </c>
       <c r="F25">
         <v>-7.9</v>
+      </c>
+      <c r="G25" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1167,10 +1155,10 @@
         <v>44204</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D26">
         <v>-2.5</v>
@@ -1180,6 +1168,9 @@
       </c>
       <c r="F26">
         <v>-5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1187,10 +1178,10 @@
         <v>44204</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D27">
         <v>-5.5</v>
@@ -1200,6 +1191,9 @@
       </c>
       <c r="F27">
         <v>14.8</v>
+      </c>
+      <c r="G27" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1207,10 +1201,10 @@
         <v>44204</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D28">
         <v>-6.5</v>
@@ -1220,6 +1214,9 @@
       </c>
       <c r="F28">
         <v>-1.3</v>
+      </c>
+      <c r="G28" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1227,10 +1224,10 @@
         <v>44204</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D29">
         <v>-1</v>
@@ -1240,6 +1237,9 @@
       </c>
       <c r="F29">
         <v>-17.7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1247,10 +1247,10 @@
         <v>44204</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D30">
         <v>5</v>
@@ -1260,6 +1260,9 @@
       </c>
       <c r="F30">
         <v>11.4</v>
+      </c>
+      <c r="G30" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1267,10 +1270,10 @@
         <v>44204</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D31">
         <v>6.5</v>
@@ -1280,6 +1283,9 @@
       </c>
       <c r="F31">
         <v>10.4</v>
+      </c>
+      <c r="G31" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1287,7 +1293,7 @@
         <v>44204</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
         <v>33</v>
@@ -1300,6 +1306,149 @@
       </c>
       <c r="F32">
         <v>-10.5</v>
+      </c>
+      <c r="G32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>44205</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>11</v>
+      </c>
+      <c r="E33">
+        <v>-3.6</v>
+      </c>
+      <c r="F33">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>44205</v>
+      </c>
+      <c r="B34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>2.8</v>
+      </c>
+      <c r="F34">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>44205</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35">
+        <v>-3</v>
+      </c>
+      <c r="E35">
+        <v>-2.8</v>
+      </c>
+      <c r="F35">
+        <v>-0.20000000000000021</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>44205</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36">
+        <v>4.5</v>
+      </c>
+      <c r="E36">
+        <v>3.7</v>
+      </c>
+      <c r="F36">
+        <v>0.79999999999999982</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>44205</v>
+      </c>
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37">
+        <v>-10.5</v>
+      </c>
+      <c r="E37">
+        <v>-26.9</v>
+      </c>
+      <c r="F37">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>44205</v>
+      </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38">
+        <v>-6</v>
+      </c>
+      <c r="E38">
+        <v>-1.8</v>
+      </c>
+      <c r="F38">
+        <v>-4.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>44205</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39">
+        <v>0.1</v>
+      </c>
+      <c r="F39">
+        <v>4.9000000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added PHI-DEN game 1/09/2021
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -8,29 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5614A4-AABC-433D-890D-9AD7767D5C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3376C2DA-603E-491F-A5CB-D5F3BF151A4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -552,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,6 +575,9 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
@@ -723,10 +716,6 @@
       <c r="G7" t="s">
         <v>38</v>
       </c>
-      <c r="J7">
-        <f>COUNTIF(G2:G32, "Yes")</f>
-        <v>17</v>
-      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -750,10 +739,6 @@
       <c r="G8" t="s">
         <v>38</v>
       </c>
-      <c r="J8">
-        <f>COUNTIF(G2:G32, "*")</f>
-        <v>31</v>
-      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -777,10 +762,6 @@
       <c r="G9" t="s">
         <v>38</v>
       </c>
-      <c r="J9">
-        <f>J7/J8</f>
-        <v>0.54838709677419351</v>
-      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
@@ -1311,143 +1292,166 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>44205</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D33">
-        <v>11</v>
+        <v>-13.5</v>
       </c>
       <c r="E33">
-        <v>-3.6</v>
+        <v>-11.1</v>
       </c>
       <c r="F33">
-        <v>14.6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-2.4</v>
+      </c>
+      <c r="G33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>44205</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D34">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E34">
-        <v>2.8</v>
+        <v>-3.6</v>
       </c>
       <c r="F34">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>44205</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D35">
-        <v>-3</v>
+        <v>5</v>
       </c>
       <c r="E35">
-        <v>-2.8</v>
+        <v>2.8</v>
       </c>
       <c r="F35">
-        <v>-0.20000000000000021</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>44205</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D36">
-        <v>4.5</v>
+        <v>-3</v>
       </c>
       <c r="E36">
-        <v>3.7</v>
+        <v>-2.8</v>
       </c>
       <c r="F36">
-        <v>0.79999999999999982</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.20000000000000021</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>44205</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D37">
-        <v>-10.5</v>
+        <v>4.5</v>
       </c>
       <c r="E37">
-        <v>-26.9</v>
+        <v>3.7</v>
       </c>
       <c r="F37">
-        <v>16.399999999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.79999999999999982</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>44205</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D38">
-        <v>-6</v>
+        <v>-10.5</v>
       </c>
       <c r="E38">
-        <v>-1.8</v>
+        <v>-26.9</v>
       </c>
       <c r="F38">
-        <v>-4.2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>44205</v>
       </c>
       <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39">
+        <v>-6</v>
+      </c>
+      <c r="E39">
+        <v>-1.8</v>
+      </c>
+      <c r="F39">
+        <v>-4.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>44205</v>
+      </c>
+      <c r="B40" t="s">
         <v>21</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>11</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <v>5</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <v>0.1</v>
       </c>
-      <c r="F39">
+      <c r="F40">
         <v>4.9000000000000004</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ran model for 01/10/2021
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31F0474-EEF3-49B3-863E-F52F88C5FD3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7094DD63-961E-44B3-A355-17393A263668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13356" yWindow="6072" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1331,6 +1331,9 @@
       <c r="F34">
         <v>14.6</v>
       </c>
+      <c r="G34" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
@@ -1351,6 +1354,9 @@
       <c r="F35">
         <v>2.2000000000000002</v>
       </c>
+      <c r="G35" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
@@ -1371,6 +1377,9 @@
       <c r="F36">
         <v>-0.20000000000000021</v>
       </c>
+      <c r="G36" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
@@ -1391,6 +1400,9 @@
       <c r="F37">
         <v>0.79999999999999982</v>
       </c>
+      <c r="G37" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
@@ -1411,6 +1423,9 @@
       <c r="F38">
         <v>16.399999999999999</v>
       </c>
+      <c r="G38" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
@@ -1431,6 +1446,9 @@
       <c r="F39">
         <v>-4.2</v>
       </c>
+      <c r="G39" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
@@ -1450,6 +1468,169 @@
       </c>
       <c r="F40">
         <v>4.9000000000000004</v>
+      </c>
+      <c r="G40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>44206</v>
+      </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41">
+        <v>8.5</v>
+      </c>
+      <c r="E41">
+        <v>9.5</v>
+      </c>
+      <c r="F41">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>44206</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42">
+        <v>-11.5</v>
+      </c>
+      <c r="E42">
+        <v>3.8</v>
+      </c>
+      <c r="F42">
+        <v>-15.3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>44206</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+      <c r="E43">
+        <v>11.7</v>
+      </c>
+      <c r="F43">
+        <v>-5.6999999999999993</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>44206</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44">
+        <v>-8.5</v>
+      </c>
+      <c r="E44">
+        <v>-13.6</v>
+      </c>
+      <c r="F44">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>44206</v>
+      </c>
+      <c r="B45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45">
+        <v>3.5</v>
+      </c>
+      <c r="E45">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="F45">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>44206</v>
+      </c>
+      <c r="B46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46">
+        <v>8</v>
+      </c>
+      <c r="E46">
+        <v>2.7</v>
+      </c>
+      <c r="F46">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>44206</v>
+      </c>
+      <c r="B47" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47">
+        <v>2.5</v>
+      </c>
+      <c r="E47">
+        <v>1.5</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>44206</v>
+      </c>
+      <c r="B48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48">
+        <v>-6.3</v>
+      </c>
+      <c r="F48">
+        <v>9.3000000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran the model for jan 11
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7094DD63-961E-44B3-A355-17393A263668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1ECD34-C893-46C4-AA10-735D58FDD591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13356" yWindow="6072" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -115,6 +115,9 @@
     <t>DAL</t>
   </si>
   <si>
+    <t>CLE</t>
+  </si>
+  <si>
     <t>UTA</t>
   </si>
   <si>
@@ -122,9 +125,6 @@
   </si>
   <si>
     <t>CHI</t>
-  </si>
-  <si>
-    <t>CLE</t>
   </si>
   <si>
     <t>OKC</t>
@@ -542,11 +542,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -584,7 +582,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2">
         <v>-4.5</v>
@@ -653,7 +651,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>-9.5</v>
@@ -676,7 +674,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6">
         <v>-9.5</v>
@@ -745,7 +743,7 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D9">
         <v>-6</v>
@@ -814,7 +812,7 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12">
         <v>7.5</v>
@@ -906,7 +904,7 @@
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D16">
         <v>-7</v>
@@ -975,7 +973,7 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D19">
         <v>-5</v>
@@ -1044,7 +1042,7 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D22">
         <v>-7</v>
@@ -1159,7 +1157,7 @@
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D27">
         <v>-5.5</v>
@@ -1274,7 +1272,7 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D32">
         <v>-9.5</v>
@@ -1355,7 +1353,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="G35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -1378,7 +1376,7 @@
         <v>-0.20000000000000021</v>
       </c>
       <c r="G36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -1389,7 +1387,7 @@
         <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D37">
         <v>4.5</v>
@@ -1412,7 +1410,7 @@
         <v>19</v>
       </c>
       <c r="C38" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D38">
         <v>-10.5</v>
@@ -1481,7 +1479,7 @@
         <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D41">
         <v>8.5</v>
@@ -1491,6 +1489,9 @@
       </c>
       <c r="F41">
         <v>-1</v>
+      </c>
+      <c r="G41" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -1501,7 +1502,7 @@
         <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D42">
         <v>-11.5</v>
@@ -1511,6 +1512,9 @@
       </c>
       <c r="F42">
         <v>-15.3</v>
+      </c>
+      <c r="G42" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -1532,6 +1536,9 @@
       <c r="F43">
         <v>-5.6999999999999993</v>
       </c>
+      <c r="G43" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
@@ -1552,6 +1559,9 @@
       <c r="F44">
         <v>5.0999999999999996</v>
       </c>
+      <c r="G44" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
@@ -1572,25 +1582,31 @@
       <c r="F45">
         <v>4.5999999999999996</v>
       </c>
+      <c r="G45" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>44206</v>
       </c>
       <c r="B46" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D46">
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="E46">
-        <v>2.7</v>
+        <v>1.5</v>
       </c>
       <c r="F46">
-        <v>5.3</v>
+        <v>1</v>
+      </c>
+      <c r="G46" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -1598,39 +1614,142 @@
         <v>44206</v>
       </c>
       <c r="B47" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C47" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D47">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="E47">
-        <v>1.5</v>
+        <v>-6.3</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G47" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
-        <v>44206</v>
+        <v>44207</v>
       </c>
       <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48">
+        <v>2.5</v>
+      </c>
+      <c r="E48">
+        <v>8.5</v>
+      </c>
+      <c r="F48">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B49" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49">
+        <v>5.5</v>
+      </c>
+      <c r="E49">
+        <v>-3.3</v>
+      </c>
+      <c r="F49">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50">
+        <v>10</v>
+      </c>
+      <c r="E50">
         <v>22</v>
       </c>
-      <c r="C48" t="s">
+      <c r="F50">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51">
+        <v>-5</v>
+      </c>
+      <c r="E51">
+        <v>-4.5</v>
+      </c>
+      <c r="F51">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52">
+        <v>-6</v>
+      </c>
+      <c r="E52">
+        <v>15.9</v>
+      </c>
+      <c r="F52">
+        <v>-21.9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s">
         <v>36</v>
       </c>
-      <c r="D48">
-        <v>3</v>
-      </c>
-      <c r="E48">
-        <v>-6.3</v>
-      </c>
-      <c r="F48">
-        <v>9.3000000000000007</v>
+      <c r="D53">
+        <v>-5</v>
+      </c>
+      <c r="E53">
+        <v>-2.8</v>
+      </c>
+      <c r="F53">
+        <v>-2.2000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added games for 1/12/2021
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -5,22 +5,32 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Documents\NBAPredictiveModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1ECD34-C893-46C4-AA10-735D58FDD591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7077E56-BED1-4B85-A620-AD0FE518D076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -118,6 +128,9 @@
     <t>CLE</t>
   </si>
   <si>
+    <t>OKC</t>
+  </si>
+  <si>
     <t>UTA</t>
   </si>
   <si>
@@ -125,9 +138,6 @@
   </si>
   <si>
     <t>CHI</t>
-  </si>
-  <si>
-    <t>OKC</t>
   </si>
   <si>
     <t>TOR</t>
@@ -542,9 +552,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -582,7 +594,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>-4.5</v>
@@ -651,7 +663,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D5">
         <v>-9.5</v>
@@ -674,7 +686,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D6">
         <v>-9.5</v>
@@ -812,7 +824,7 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>7.5</v>
@@ -835,7 +847,7 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D13">
         <v>-8</v>
@@ -904,7 +916,7 @@
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D16">
         <v>-7</v>
@@ -1042,7 +1054,7 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D22">
         <v>-7</v>
@@ -1134,7 +1146,7 @@
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D26">
         <v>-2.5</v>
@@ -1157,7 +1169,7 @@
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D27">
         <v>-5.5</v>
@@ -1272,7 +1284,7 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D32">
         <v>-9.5</v>
@@ -1387,7 +1399,7 @@
         <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D37">
         <v>4.5</v>
@@ -1479,7 +1491,7 @@
         <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D41">
         <v>8.5</v>
@@ -1502,7 +1514,7 @@
         <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D42">
         <v>-11.5</v>
@@ -1548,7 +1560,7 @@
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D44">
         <v>-8.5</v>
@@ -1594,7 +1606,7 @@
         <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D46">
         <v>2.5</v>
@@ -1651,8 +1663,11 @@
       <c r="F48">
         <v>-6</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>44207</v>
       </c>
@@ -1671,8 +1686,11 @@
       <c r="F49">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>44207</v>
       </c>
@@ -1691,8 +1709,11 @@
       <c r="F50">
         <v>-12</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>44207</v>
       </c>
@@ -1711,8 +1732,11 @@
       <c r="F51">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>44207</v>
       </c>
@@ -1731,8 +1755,11 @@
       <c r="F52">
         <v>-21.9</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>44207</v>
       </c>
@@ -1750,6 +1777,129 @@
       </c>
       <c r="F53">
         <v>-2.2000000000000002</v>
+      </c>
+      <c r="G53" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54">
+        <v>-8</v>
+      </c>
+      <c r="E54">
+        <v>2.5</v>
+      </c>
+      <c r="F54">
+        <v>-10.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55">
+        <v>-1</v>
+      </c>
+      <c r="E55">
+        <v>-8.1999999999999993</v>
+      </c>
+      <c r="F55">
+        <v>7.1999999999999993</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56">
+        <v>12</v>
+      </c>
+      <c r="E56">
+        <v>14</v>
+      </c>
+      <c r="F56">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B57" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" t="s">
+        <v>34</v>
+      </c>
+      <c r="D57">
+        <v>2.5</v>
+      </c>
+      <c r="E57">
+        <v>-4.8</v>
+      </c>
+      <c r="F57">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58">
+        <v>4.5</v>
+      </c>
+      <c r="E58">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F58">
+        <v>0.40000000000000041</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B59" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59">
+        <v>-3</v>
+      </c>
+      <c r="E59">
+        <v>-2.8</v>
+      </c>
+      <c r="F59">
+        <v>-0.20000000000000021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added games for 1/13/2021
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -8,29 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7077E56-BED1-4B85-A620-AD0FE518D076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3C2364-033D-4338-8DA2-D69B20E4B9D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -552,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1801,6 +1791,9 @@
       <c r="F54">
         <v>-10.5</v>
       </c>
+      <c r="G54" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
@@ -1821,6 +1814,9 @@
       <c r="F55">
         <v>7.1999999999999993</v>
       </c>
+      <c r="G55" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
@@ -1841,6 +1837,9 @@
       <c r="F56">
         <v>-2</v>
       </c>
+      <c r="G56" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
@@ -1861,6 +1860,9 @@
       <c r="F57">
         <v>7.3</v>
       </c>
+      <c r="G57" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
@@ -1881,6 +1883,9 @@
       <c r="F58">
         <v>0.40000000000000041</v>
       </c>
+      <c r="G58" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
@@ -1900,6 +1905,169 @@
       </c>
       <c r="F59">
         <v>-0.20000000000000021</v>
+      </c>
+      <c r="G59" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60">
+        <v>10.5</v>
+      </c>
+      <c r="E60">
+        <v>23.3</v>
+      </c>
+      <c r="F60">
+        <v>-12.8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B61" t="s">
+        <v>28</v>
+      </c>
+      <c r="C61" t="s">
+        <v>30</v>
+      </c>
+      <c r="D61">
+        <v>4</v>
+      </c>
+      <c r="E61">
+        <v>-0.2</v>
+      </c>
+      <c r="F61">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62">
+        <v>6</v>
+      </c>
+      <c r="E62">
+        <v>26.5</v>
+      </c>
+      <c r="F62">
+        <v>-20.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B63" t="s">
+        <v>29</v>
+      </c>
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63">
+        <v>-3.5</v>
+      </c>
+      <c r="E63">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="F63">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B64" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64">
+        <v>9</v>
+      </c>
+      <c r="E64">
+        <v>8.1</v>
+      </c>
+      <c r="F64">
+        <v>0.90000000000000036</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B65" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" t="s">
+        <v>16</v>
+      </c>
+      <c r="D65">
+        <v>-5.5</v>
+      </c>
+      <c r="E65">
+        <v>-7.6</v>
+      </c>
+      <c r="F65">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66">
+        <v>-6</v>
+      </c>
+      <c r="E66">
+        <v>-4.8</v>
+      </c>
+      <c r="F66">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B67" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67">
+        <v>4.5</v>
+      </c>
+      <c r="E67">
+        <v>-3</v>
+      </c>
+      <c r="F67">
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran model for 1/14/2021
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3C2364-033D-4338-8DA2-D69B20E4B9D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2587AD2D-6BBB-46CD-A6C4-421CA62024F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -121,10 +121,10 @@
     <t>OKC</t>
   </si>
   <si>
+    <t>SAS</t>
+  </si>
+  <si>
     <t>UTA</t>
-  </si>
-  <si>
-    <t>SAS</t>
   </si>
   <si>
     <t>CHI</t>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,7 +584,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2">
         <v>-4.5</v>
@@ -653,7 +653,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>-9.5</v>
@@ -814,7 +814,7 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12">
         <v>7.5</v>
@@ -1044,7 +1044,7 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22">
         <v>-7</v>
@@ -1159,7 +1159,7 @@
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D27">
         <v>-5.5</v>
@@ -1389,7 +1389,7 @@
         <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D37">
         <v>4.5</v>
@@ -1481,7 +1481,7 @@
         <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D41">
         <v>8.5</v>
@@ -1596,7 +1596,7 @@
         <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D46">
         <v>2.5</v>
@@ -1826,7 +1826,7 @@
         <v>31</v>
       </c>
       <c r="C56" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D56">
         <v>12</v>
@@ -1849,7 +1849,7 @@
         <v>32</v>
       </c>
       <c r="C57" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D57">
         <v>2.5</v>
@@ -1929,6 +1929,9 @@
       <c r="F60">
         <v>-12.8</v>
       </c>
+      <c r="G60" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
@@ -1949,6 +1952,9 @@
       <c r="F61">
         <v>4.2</v>
       </c>
+      <c r="G61" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
@@ -1969,6 +1975,9 @@
       <c r="F62">
         <v>-20.5</v>
       </c>
+      <c r="G62" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
@@ -1989,6 +1998,9 @@
       <c r="F63">
         <v>-1.2</v>
       </c>
+      <c r="G63" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
@@ -2009,65 +2021,154 @@
       <c r="F64">
         <v>0.90000000000000036</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>44209</v>
       </c>
       <c r="B65" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C65" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D65">
-        <v>-5.5</v>
+        <v>-6</v>
       </c>
       <c r="E65">
-        <v>-7.6</v>
+        <v>-4.8</v>
       </c>
       <c r="F65">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-1.2</v>
+      </c>
+      <c r="G65" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>44209</v>
       </c>
       <c r="B66" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66">
+        <v>4.5</v>
+      </c>
+      <c r="E66">
+        <v>-3</v>
+      </c>
+      <c r="F66">
+        <v>7.5</v>
+      </c>
+      <c r="G66" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B67" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67">
+        <v>-7</v>
+      </c>
+      <c r="E67">
+        <v>0.6</v>
+      </c>
+      <c r="F67">
+        <v>-7.6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B68" t="s">
+        <v>33</v>
+      </c>
+      <c r="C68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68">
+        <v>-7</v>
+      </c>
+      <c r="E68">
+        <v>2.6</v>
+      </c>
+      <c r="F68">
+        <v>-9.6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B69" t="s">
+        <v>28</v>
+      </c>
+      <c r="C69" t="s">
+        <v>36</v>
+      </c>
+      <c r="D69">
         <v>10</v>
       </c>
-      <c r="C66" t="s">
-        <v>18</v>
-      </c>
-      <c r="D66">
-        <v>-6</v>
-      </c>
-      <c r="E66">
-        <v>-4.8</v>
-      </c>
-      <c r="F66">
-        <v>-1.2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="2">
-        <v>44209</v>
-      </c>
-      <c r="B67" t="s">
-        <v>21</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="E69">
+        <v>4.3</v>
+      </c>
+      <c r="F69">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" t="s">
+        <v>22</v>
+      </c>
+      <c r="D70">
+        <v>-4.5</v>
+      </c>
+      <c r="E70">
+        <v>-3.4</v>
+      </c>
+      <c r="F70">
+        <v>-1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B71" t="s">
         <v>11</v>
       </c>
-      <c r="D67">
-        <v>4.5</v>
-      </c>
-      <c r="E67">
+      <c r="C71" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71">
         <v>-3</v>
       </c>
-      <c r="F67">
-        <v>7.5</v>
+      <c r="E71">
+        <v>-3.3</v>
+      </c>
+      <c r="F71">
+        <v>0.29999999999999982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran model jan 15
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2587AD2D-6BBB-46CD-A6C4-421CA62024F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -142,11 +136,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,14 +204,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -264,7 +250,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -296,27 +282,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -348,24 +316,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -541,19 +491,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="I71" sqref="I71"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,7 +521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>44201</v>
       </c>
@@ -599,7 +544,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>44201</v>
       </c>
@@ -622,7 +567,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>44201</v>
       </c>
@@ -645,7 +590,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>44201</v>
       </c>
@@ -659,7 +604,7 @@
         <v>-9.5</v>
       </c>
       <c r="E5">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="F5">
         <v>-11.8</v>
@@ -668,7 +613,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>44201</v>
       </c>
@@ -685,13 +630,13 @@
         <v>7.4</v>
       </c>
       <c r="F6">
-        <v>-16.899999999999999</v>
+        <v>-16.9</v>
       </c>
       <c r="G6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>44202</v>
       </c>
@@ -714,7 +659,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>44202</v>
       </c>
@@ -737,7 +682,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>44202</v>
       </c>
@@ -754,13 +699,13 @@
         <v>-6.2</v>
       </c>
       <c r="F9">
-        <v>0.20000000000000021</v>
+        <v>0.2000000000000002</v>
       </c>
       <c r="G9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>44202</v>
       </c>
@@ -783,7 +728,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>44202</v>
       </c>
@@ -806,7 +751,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>44202</v>
       </c>
@@ -829,7 +774,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>44202</v>
       </c>
@@ -852,7 +797,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14" s="2">
         <v>44202</v>
       </c>
@@ -875,7 +820,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
         <v>44202</v>
       </c>
@@ -898,7 +843,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" s="2">
         <v>44202</v>
       </c>
@@ -921,7 +866,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
         <v>44202</v>
       </c>
@@ -944,7 +889,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18" s="2">
         <v>44203</v>
       </c>
@@ -967,7 +912,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
         <v>44203</v>
       </c>
@@ -990,7 +935,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20" s="2">
         <v>44203</v>
       </c>
@@ -1004,7 +949,7 @@
         <v>-10</v>
       </c>
       <c r="E20">
-        <v>-4.4000000000000004</v>
+        <v>-4.4</v>
       </c>
       <c r="F20">
         <v>-5.6</v>
@@ -1013,7 +958,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
         <v>44203</v>
       </c>
@@ -1036,7 +981,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22" s="2">
         <v>44203</v>
       </c>
@@ -1053,13 +998,13 @@
         <v>-6.2</v>
       </c>
       <c r="F22">
-        <v>-0.79999999999999982</v>
+        <v>-0.7999999999999998</v>
       </c>
       <c r="G22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23" s="2">
         <v>44204</v>
       </c>
@@ -1082,7 +1027,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24" s="2">
         <v>44204</v>
       </c>
@@ -1105,7 +1050,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25" s="2">
         <v>44204</v>
       </c>
@@ -1128,7 +1073,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26" s="2">
         <v>44204</v>
       </c>
@@ -1151,7 +1096,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="A27" s="2">
         <v>44204</v>
       </c>
@@ -1174,7 +1119,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28" s="2">
         <v>44204</v>
       </c>
@@ -1197,7 +1142,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="A29" s="2">
         <v>44204</v>
       </c>
@@ -1220,7 +1165,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30" s="2">
         <v>44204</v>
       </c>
@@ -1243,7 +1188,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7">
       <c r="A31" s="2">
         <v>44204</v>
       </c>
@@ -1266,7 +1211,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7">
       <c r="A32" s="2">
         <v>44204</v>
       </c>
@@ -1289,7 +1234,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7">
       <c r="A33" s="2">
         <v>44205</v>
       </c>
@@ -1312,7 +1257,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7">
       <c r="A34" s="2">
         <v>44205</v>
       </c>
@@ -1335,7 +1280,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7">
       <c r="A35" s="2">
         <v>44205</v>
       </c>
@@ -1352,13 +1297,13 @@
         <v>2.8</v>
       </c>
       <c r="F35">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="G35" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7">
       <c r="A36" s="2">
         <v>44205</v>
       </c>
@@ -1375,13 +1320,13 @@
         <v>-2.8</v>
       </c>
       <c r="F36">
-        <v>-0.20000000000000021</v>
+        <v>-0.2000000000000002</v>
       </c>
       <c r="G36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7">
       <c r="A37" s="2">
         <v>44205</v>
       </c>
@@ -1398,13 +1343,13 @@
         <v>3.7</v>
       </c>
       <c r="F37">
-        <v>0.79999999999999982</v>
+        <v>0.7999999999999998</v>
       </c>
       <c r="G37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7">
       <c r="A38" s="2">
         <v>44205</v>
       </c>
@@ -1421,13 +1366,13 @@
         <v>-26.9</v>
       </c>
       <c r="F38">
-        <v>16.399999999999999</v>
+        <v>16.4</v>
       </c>
       <c r="G38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7">
       <c r="A39" s="2">
         <v>44205</v>
       </c>
@@ -1450,7 +1395,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7">
       <c r="A40" s="2">
         <v>44205</v>
       </c>
@@ -1467,13 +1412,13 @@
         <v>0.1</v>
       </c>
       <c r="F40">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="G40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7">
       <c r="A41" s="2">
         <v>44206</v>
       </c>
@@ -1496,7 +1441,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7">
       <c r="A42" s="2">
         <v>44206</v>
       </c>
@@ -1519,7 +1464,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7">
       <c r="A43" s="2">
         <v>44206</v>
       </c>
@@ -1536,13 +1481,13 @@
         <v>11.7</v>
       </c>
       <c r="F43">
-        <v>-5.6999999999999993</v>
+        <v>-5.699999999999999</v>
       </c>
       <c r="G43" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7">
       <c r="A44" s="2">
         <v>44206</v>
       </c>
@@ -1559,13 +1504,13 @@
         <v>-13.6</v>
       </c>
       <c r="F44">
-        <v>5.0999999999999996</v>
+        <v>5.1</v>
       </c>
       <c r="G44" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7">
       <c r="A45" s="2">
         <v>44206</v>
       </c>
@@ -1579,16 +1524,16 @@
         <v>3.5</v>
       </c>
       <c r="E45">
-        <v>-1.1000000000000001</v>
+        <v>-1.1</v>
       </c>
       <c r="F45">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="G45" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7">
       <c r="A46" s="2">
         <v>44206</v>
       </c>
@@ -1611,7 +1556,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7">
       <c r="A47" s="2">
         <v>44206</v>
       </c>
@@ -1628,13 +1573,13 @@
         <v>-6.3</v>
       </c>
       <c r="F47">
-        <v>9.3000000000000007</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="G47" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7">
       <c r="A48" s="2">
         <v>44207</v>
       </c>
@@ -1657,7 +1602,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7">
       <c r="A49" s="2">
         <v>44207</v>
       </c>
@@ -1674,13 +1619,13 @@
         <v>-3.3</v>
       </c>
       <c r="F49">
-        <v>8.8000000000000007</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="G49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7">
       <c r="A50" s="2">
         <v>44207</v>
       </c>
@@ -1703,7 +1648,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7">
       <c r="A51" s="2">
         <v>44207</v>
       </c>
@@ -1726,7 +1671,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7">
       <c r="A52" s="2">
         <v>44207</v>
       </c>
@@ -1749,7 +1694,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7">
       <c r="A53" s="2">
         <v>44207</v>
       </c>
@@ -1766,13 +1711,13 @@
         <v>-2.8</v>
       </c>
       <c r="F53">
-        <v>-2.2000000000000002</v>
+        <v>-2.2</v>
       </c>
       <c r="G53" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7">
       <c r="A54" s="2">
         <v>44208</v>
       </c>
@@ -1795,7 +1740,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7">
       <c r="A55" s="2">
         <v>44208</v>
       </c>
@@ -1809,16 +1754,16 @@
         <v>-1</v>
       </c>
       <c r="E55">
-        <v>-8.1999999999999993</v>
+        <v>-8.199999999999999</v>
       </c>
       <c r="F55">
-        <v>7.1999999999999993</v>
+        <v>7.199999999999999</v>
       </c>
       <c r="G55" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7">
       <c r="A56" s="2">
         <v>44208</v>
       </c>
@@ -1841,7 +1786,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7">
       <c r="A57" s="2">
         <v>44208</v>
       </c>
@@ -1864,7 +1809,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7">
       <c r="A58" s="2">
         <v>44208</v>
       </c>
@@ -1878,16 +1823,16 @@
         <v>4.5</v>
       </c>
       <c r="E58">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="F58">
-        <v>0.40000000000000041</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="G58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7">
       <c r="A59" s="2">
         <v>44208</v>
       </c>
@@ -1904,13 +1849,13 @@
         <v>-2.8</v>
       </c>
       <c r="F59">
-        <v>-0.20000000000000021</v>
+        <v>-0.2000000000000002</v>
       </c>
       <c r="G59" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7">
       <c r="A60" s="2">
         <v>44209</v>
       </c>
@@ -1933,7 +1878,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7">
       <c r="A61" s="2">
         <v>44209</v>
       </c>
@@ -1956,7 +1901,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7">
       <c r="A62" s="2">
         <v>44209</v>
       </c>
@@ -1979,7 +1924,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7">
       <c r="A63" s="2">
         <v>44209</v>
       </c>
@@ -1993,7 +1938,7 @@
         <v>-3.5</v>
       </c>
       <c r="E63">
-        <v>-2.2999999999999998</v>
+        <v>-2.3</v>
       </c>
       <c r="F63">
         <v>-1.2</v>
@@ -2002,7 +1947,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7">
       <c r="A64" s="2">
         <v>44209</v>
       </c>
@@ -2019,13 +1964,13 @@
         <v>8.1</v>
       </c>
       <c r="F64">
-        <v>0.90000000000000036</v>
+        <v>0.9000000000000004</v>
       </c>
       <c r="G64" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7">
       <c r="A65" s="2">
         <v>44209</v>
       </c>
@@ -2048,7 +1993,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7">
       <c r="A66" s="2">
         <v>44209</v>
       </c>
@@ -2071,7 +2016,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7">
       <c r="A67" s="2">
         <v>44210</v>
       </c>
@@ -2090,8 +2035,11 @@
       <c r="F67">
         <v>-7.6</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G67" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" s="2">
         <v>44210</v>
       </c>
@@ -2110,8 +2058,11 @@
       <c r="F68">
         <v>-9.6</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G68" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="2">
         <v>44210</v>
       </c>
@@ -2130,8 +2081,11 @@
       <c r="F69">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G69" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" s="2">
         <v>44210</v>
       </c>
@@ -2148,10 +2102,13 @@
         <v>-3.4</v>
       </c>
       <c r="F70">
-        <v>-1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-1.1</v>
+      </c>
+      <c r="G70" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="2">
         <v>44210</v>
       </c>
@@ -2168,7 +2125,170 @@
         <v>-3.3</v>
       </c>
       <c r="F71">
-        <v>0.29999999999999982</v>
+        <v>0.2999999999999998</v>
+      </c>
+      <c r="G71" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="2">
+        <v>44211</v>
+      </c>
+      <c r="B72" t="s">
+        <v>31</v>
+      </c>
+      <c r="C72" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="E72">
+        <v>2.1</v>
+      </c>
+      <c r="F72">
+        <v>-0.1000000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="2">
+        <v>44211</v>
+      </c>
+      <c r="B73" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73">
+        <v>-2.5</v>
+      </c>
+      <c r="E73">
+        <v>-8.4</v>
+      </c>
+      <c r="F73">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="2">
+        <v>44211</v>
+      </c>
+      <c r="B74" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" t="s">
+        <v>30</v>
+      </c>
+      <c r="D74">
+        <v>-7</v>
+      </c>
+      <c r="E74">
+        <v>-13.6</v>
+      </c>
+      <c r="F74">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="2">
+        <v>44211</v>
+      </c>
+      <c r="B75" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75" t="s">
+        <v>35</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>10.9</v>
+      </c>
+      <c r="F75">
+        <v>-10.9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="2">
+        <v>44211</v>
+      </c>
+      <c r="B76" t="s">
+        <v>29</v>
+      </c>
+      <c r="C76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76">
+        <v>-1</v>
+      </c>
+      <c r="E76">
+        <v>-0.2</v>
+      </c>
+      <c r="F76">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="2">
+        <v>44211</v>
+      </c>
+      <c r="B77" t="s">
+        <v>34</v>
+      </c>
+      <c r="C77" t="s">
+        <v>16</v>
+      </c>
+      <c r="D77">
+        <v>-6</v>
+      </c>
+      <c r="E77">
+        <v>-9.6</v>
+      </c>
+      <c r="F77">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="2">
+        <v>44211</v>
+      </c>
+      <c r="B78" t="s">
+        <v>23</v>
+      </c>
+      <c r="C78" t="s">
+        <v>18</v>
+      </c>
+      <c r="D78">
+        <v>-10</v>
+      </c>
+      <c r="E78">
+        <v>-12.7</v>
+      </c>
+      <c r="F78">
+        <v>2.699999999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="2">
+        <v>44211</v>
+      </c>
+      <c r="B79" t="s">
+        <v>21</v>
+      </c>
+      <c r="C79" t="s">
+        <v>10</v>
+      </c>
+      <c r="D79">
+        <v>7</v>
+      </c>
+      <c r="E79">
+        <v>-5.8</v>
+      </c>
+      <c r="F79">
+        <v>12.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran model for jan 16
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Documents\NBAPredictiveModel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80025F6-E6FB-4980-B7DD-90C1C7AC2A1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -121,10 +127,10 @@
     <t>UTA</t>
   </si>
   <si>
+    <t>TOR</t>
+  </si>
+  <si>
     <t>CHI</t>
-  </si>
-  <si>
-    <t>TOR</t>
   </si>
   <si>
     <t>No</t>
@@ -136,11 +142,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +210,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -250,7 +264,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -282,9 +296,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -316,6 +348,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -491,14 +541,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="L93" sqref="L93"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,7 +576,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44201</v>
       </c>
@@ -544,7 +599,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44201</v>
       </c>
@@ -567,7 +622,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44201</v>
       </c>
@@ -590,7 +645,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44201</v>
       </c>
@@ -604,7 +659,7 @@
         <v>-9.5</v>
       </c>
       <c r="E5">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F5">
         <v>-11.8</v>
@@ -613,7 +668,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44201</v>
       </c>
@@ -621,7 +676,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6">
         <v>-9.5</v>
@@ -630,13 +685,13 @@
         <v>7.4</v>
       </c>
       <c r="F6">
-        <v>-16.9</v>
+        <v>-16.899999999999999</v>
       </c>
       <c r="G6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>44202</v>
       </c>
@@ -659,7 +714,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>44202</v>
       </c>
@@ -682,7 +737,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>44202</v>
       </c>
@@ -699,13 +754,13 @@
         <v>-6.2</v>
       </c>
       <c r="F9">
-        <v>0.2000000000000002</v>
+        <v>0.20000000000000021</v>
       </c>
       <c r="G9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>44202</v>
       </c>
@@ -728,7 +783,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44202</v>
       </c>
@@ -751,7 +806,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>44202</v>
       </c>
@@ -774,7 +829,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44202</v>
       </c>
@@ -797,7 +852,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>44202</v>
       </c>
@@ -820,7 +875,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>44202</v>
       </c>
@@ -828,7 +883,7 @@
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15">
         <v>-3</v>
@@ -843,7 +898,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>44202</v>
       </c>
@@ -851,7 +906,7 @@
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D16">
         <v>-7</v>
@@ -866,7 +921,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44202</v>
       </c>
@@ -889,7 +944,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>44203</v>
       </c>
@@ -912,7 +967,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>44203</v>
       </c>
@@ -935,7 +990,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>44203</v>
       </c>
@@ -949,7 +1004,7 @@
         <v>-10</v>
       </c>
       <c r="E20">
-        <v>-4.4</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="F20">
         <v>-5.6</v>
@@ -958,7 +1013,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>44203</v>
       </c>
@@ -981,7 +1036,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>44203</v>
       </c>
@@ -998,13 +1053,13 @@
         <v>-6.2</v>
       </c>
       <c r="F22">
-        <v>-0.7999999999999998</v>
+        <v>-0.79999999999999982</v>
       </c>
       <c r="G22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>44204</v>
       </c>
@@ -1027,7 +1082,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>44204</v>
       </c>
@@ -1050,7 +1105,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>44204</v>
       </c>
@@ -1073,7 +1128,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>44204</v>
       </c>
@@ -1096,7 +1151,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>44204</v>
       </c>
@@ -1119,7 +1174,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>44204</v>
       </c>
@@ -1142,7 +1197,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>44204</v>
       </c>
@@ -1165,7 +1220,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>44204</v>
       </c>
@@ -1173,7 +1228,7 @@
         <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30">
         <v>5</v>
@@ -1188,7 +1243,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>44204</v>
       </c>
@@ -1211,7 +1266,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>44204</v>
       </c>
@@ -1219,7 +1274,7 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D32">
         <v>-9.5</v>
@@ -1234,7 +1289,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>44205</v>
       </c>
@@ -1257,7 +1312,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>44205</v>
       </c>
@@ -1280,7 +1335,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>44205</v>
       </c>
@@ -1297,13 +1352,13 @@
         <v>2.8</v>
       </c>
       <c r="F35">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G35" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>44205</v>
       </c>
@@ -1320,13 +1375,13 @@
         <v>-2.8</v>
       </c>
       <c r="F36">
-        <v>-0.2000000000000002</v>
+        <v>-0.20000000000000021</v>
       </c>
       <c r="G36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>44205</v>
       </c>
@@ -1343,13 +1398,13 @@
         <v>3.7</v>
       </c>
       <c r="F37">
-        <v>0.7999999999999998</v>
+        <v>0.79999999999999982</v>
       </c>
       <c r="G37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>44205</v>
       </c>
@@ -1366,13 +1421,13 @@
         <v>-26.9</v>
       </c>
       <c r="F38">
-        <v>16.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="G38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>44205</v>
       </c>
@@ -1395,7 +1450,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>44205</v>
       </c>
@@ -1412,13 +1467,13 @@
         <v>0.1</v>
       </c>
       <c r="F40">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>44206</v>
       </c>
@@ -1441,7 +1496,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>44206</v>
       </c>
@@ -1449,7 +1504,7 @@
         <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D42">
         <v>-11.5</v>
@@ -1464,7 +1519,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>44206</v>
       </c>
@@ -1481,13 +1536,13 @@
         <v>11.7</v>
       </c>
       <c r="F43">
-        <v>-5.699999999999999</v>
+        <v>-5.6999999999999993</v>
       </c>
       <c r="G43" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>44206</v>
       </c>
@@ -1504,13 +1559,13 @@
         <v>-13.6</v>
       </c>
       <c r="F44">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G44" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44206</v>
       </c>
@@ -1524,16 +1579,16 @@
         <v>3.5</v>
       </c>
       <c r="E45">
-        <v>-1.1</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="F45">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="G45" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>44206</v>
       </c>
@@ -1556,7 +1611,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>44206</v>
       </c>
@@ -1564,7 +1619,7 @@
         <v>22</v>
       </c>
       <c r="C47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D47">
         <v>3</v>
@@ -1573,13 +1628,13 @@
         <v>-6.3</v>
       </c>
       <c r="F47">
-        <v>9.300000000000001</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="G47" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>44207</v>
       </c>
@@ -1602,7 +1657,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>44207</v>
       </c>
@@ -1619,13 +1674,13 @@
         <v>-3.3</v>
       </c>
       <c r="F49">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="G49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>44207</v>
       </c>
@@ -1648,7 +1703,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>44207</v>
       </c>
@@ -1671,7 +1726,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>44207</v>
       </c>
@@ -1694,7 +1749,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>44207</v>
       </c>
@@ -1702,7 +1757,7 @@
         <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D53">
         <v>-5</v>
@@ -1711,13 +1766,13 @@
         <v>-2.8</v>
       </c>
       <c r="F53">
-        <v>-2.2</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="G53" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>44208</v>
       </c>
@@ -1740,7 +1795,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>44208</v>
       </c>
@@ -1754,16 +1809,16 @@
         <v>-1</v>
       </c>
       <c r="E55">
-        <v>-8.199999999999999</v>
+        <v>-8.1999999999999993</v>
       </c>
       <c r="F55">
-        <v>7.199999999999999</v>
+        <v>7.1999999999999993</v>
       </c>
       <c r="G55" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>44208</v>
       </c>
@@ -1786,7 +1841,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>44208</v>
       </c>
@@ -1809,7 +1864,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>44208</v>
       </c>
@@ -1823,16 +1878,16 @@
         <v>4.5</v>
       </c>
       <c r="E58">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F58">
-        <v>0.4000000000000004</v>
+        <v>0.40000000000000041</v>
       </c>
       <c r="G58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>44208</v>
       </c>
@@ -1849,13 +1904,13 @@
         <v>-2.8</v>
       </c>
       <c r="F59">
-        <v>-0.2000000000000002</v>
+        <v>-0.20000000000000021</v>
       </c>
       <c r="G59" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>44209</v>
       </c>
@@ -1878,7 +1933,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>44209</v>
       </c>
@@ -1901,7 +1956,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>44209</v>
       </c>
@@ -1924,7 +1979,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>44209</v>
       </c>
@@ -1938,7 +1993,7 @@
         <v>-3.5</v>
       </c>
       <c r="E63">
-        <v>-2.3</v>
+        <v>-2.2999999999999998</v>
       </c>
       <c r="F63">
         <v>-1.2</v>
@@ -1947,7 +2002,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>44209</v>
       </c>
@@ -1964,13 +2019,13 @@
         <v>8.1</v>
       </c>
       <c r="F64">
-        <v>0.9000000000000004</v>
+        <v>0.90000000000000036</v>
       </c>
       <c r="G64" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>44209</v>
       </c>
@@ -1993,7 +2048,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>44209</v>
       </c>
@@ -2016,7 +2071,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>44210</v>
       </c>
@@ -2039,7 +2094,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>44210</v>
       </c>
@@ -2062,7 +2117,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>44210</v>
       </c>
@@ -2070,7 +2125,7 @@
         <v>28</v>
       </c>
       <c r="C69" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D69">
         <v>10</v>
@@ -2085,7 +2140,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>44210</v>
       </c>
@@ -2102,13 +2157,13 @@
         <v>-3.4</v>
       </c>
       <c r="F70">
-        <v>-1.1</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="G70" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>44210</v>
       </c>
@@ -2125,13 +2180,13 @@
         <v>-3.3</v>
       </c>
       <c r="F71">
-        <v>0.2999999999999998</v>
+        <v>0.29999999999999982</v>
       </c>
       <c r="G71" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>44211</v>
       </c>
@@ -2150,8 +2205,11 @@
       <c r="F72">
         <v>-0.1000000000000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:7">
+      <c r="G72" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>44211</v>
       </c>
@@ -2170,8 +2228,11 @@
       <c r="F73">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="74" spans="1:7">
+      <c r="G73" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>44211</v>
       </c>
@@ -2190,8 +2251,11 @@
       <c r="F74">
         <v>6.6</v>
       </c>
-    </row>
-    <row r="75" spans="1:7">
+      <c r="G74" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>44211</v>
       </c>
@@ -2199,7 +2263,7 @@
         <v>32</v>
       </c>
       <c r="C75" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -2210,85 +2274,197 @@
       <c r="F75">
         <v>-10.9</v>
       </c>
-    </row>
-    <row r="76" spans="1:7">
+      <c r="G75" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>44211</v>
       </c>
       <c r="B76" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C76" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D76">
-        <v>-1</v>
+        <v>-6</v>
       </c>
       <c r="E76">
-        <v>-0.2</v>
+        <v>-9.6</v>
       </c>
       <c r="F76">
-        <v>-0.8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
+        <v>3.6</v>
+      </c>
+      <c r="G76" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>44211</v>
       </c>
       <c r="B77" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C77" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D77">
-        <v>-6</v>
+        <v>-10</v>
       </c>
       <c r="E77">
-        <v>-9.6</v>
+        <v>-12.7</v>
       </c>
       <c r="F77">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
+        <v>2.6999999999999988</v>
+      </c>
+      <c r="G77" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>44211</v>
       </c>
       <c r="B78" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C78" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D78">
-        <v>-10</v>
+        <v>7</v>
       </c>
       <c r="E78">
-        <v>-12.7</v>
+        <v>-5.8</v>
       </c>
       <c r="F78">
-        <v>2.699999999999999</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
+        <v>12.8</v>
+      </c>
+      <c r="G78" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
-        <v>44211</v>
+        <v>44212</v>
       </c>
       <c r="B79" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C79" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D79">
+        <v>-7</v>
+      </c>
+      <c r="E79">
+        <v>5.6</v>
+      </c>
+      <c r="F79">
+        <v>-12.6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" s="2">
+        <v>44212</v>
+      </c>
+      <c r="B80" t="s">
         <v>7</v>
       </c>
-      <c r="E79">
-        <v>-5.8</v>
-      </c>
-      <c r="F79">
-        <v>12.8</v>
+      <c r="C80" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80">
+        <v>-8</v>
+      </c>
+      <c r="E80">
+        <v>-20.9</v>
+      </c>
+      <c r="F80">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="2">
+        <v>44212</v>
+      </c>
+      <c r="B81" t="s">
+        <v>35</v>
+      </c>
+      <c r="C81" t="s">
+        <v>28</v>
+      </c>
+      <c r="D81">
+        <v>-7</v>
+      </c>
+      <c r="E81">
+        <v>-4</v>
+      </c>
+      <c r="F81">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="2">
+        <v>44212</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82">
+        <v>-1.5</v>
+      </c>
+      <c r="E82">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F82">
+        <v>-9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="2">
+        <v>44212</v>
+      </c>
+      <c r="B83" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" t="s">
+        <v>24</v>
+      </c>
+      <c r="D83">
+        <v>-5</v>
+      </c>
+      <c r="E83">
+        <v>-18.600000000000001</v>
+      </c>
+      <c r="F83">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="2">
+        <v>44212</v>
+      </c>
+      <c r="B84" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84" t="s">
+        <v>16</v>
+      </c>
+      <c r="D84">
+        <v>-5</v>
+      </c>
+      <c r="E84">
+        <v>-12.4</v>
+      </c>
+      <c r="F84">
+        <v>7.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added games for 1/17/2021
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Documents\NBAPredictiveModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80025F6-E6FB-4980-B7DD-90C1C7AC2A1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BE31F3-40C5-49E5-BACC-25A04642F32F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="L93" sqref="L93"/>
+      <selection activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2366,6 +2366,9 @@
       <c r="F79">
         <v>-12.6</v>
       </c>
+      <c r="G79" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
@@ -2386,8 +2389,11 @@
       <c r="F80">
         <v>12.9</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G80" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>44212</v>
       </c>
@@ -2406,8 +2412,11 @@
       <c r="F81">
         <v>-3</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G81" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>44212</v>
       </c>
@@ -2426,8 +2435,11 @@
       <c r="F82">
         <v>-9.6999999999999993</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G82" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>44212</v>
       </c>
@@ -2446,8 +2458,11 @@
       <c r="F83">
         <v>13.6</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G83" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>44212</v>
       </c>
@@ -2465,6 +2480,129 @@
       </c>
       <c r="F84">
         <v>7.4</v>
+      </c>
+      <c r="G84" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="2">
+        <v>44213</v>
+      </c>
+      <c r="B85" t="s">
+        <v>25</v>
+      </c>
+      <c r="C85" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85">
+        <v>-7</v>
+      </c>
+      <c r="E85">
+        <v>-18</v>
+      </c>
+      <c r="F85">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" s="2">
+        <v>44213</v>
+      </c>
+      <c r="B86" t="s">
+        <v>30</v>
+      </c>
+      <c r="C86" t="s">
+        <v>36</v>
+      </c>
+      <c r="D86">
+        <v>-7</v>
+      </c>
+      <c r="E86">
+        <v>13.8</v>
+      </c>
+      <c r="F86">
+        <v>-20.8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" s="2">
+        <v>44213</v>
+      </c>
+      <c r="B87" t="s">
+        <v>32</v>
+      </c>
+      <c r="C87" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87">
+        <v>2.5</v>
+      </c>
+      <c r="E87">
+        <v>3.7</v>
+      </c>
+      <c r="F87">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88" s="2">
+        <v>44213</v>
+      </c>
+      <c r="B88" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" t="s">
+        <v>34</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>0.3</v>
+      </c>
+      <c r="F88">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" s="2">
+        <v>44213</v>
+      </c>
+      <c r="B89" t="s">
+        <v>21</v>
+      </c>
+      <c r="C89" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89">
+        <v>2.5</v>
+      </c>
+      <c r="E89">
+        <v>-10.7</v>
+      </c>
+      <c r="F89">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90" s="2">
+        <v>44213</v>
+      </c>
+      <c r="B90" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" t="s">
+        <v>12</v>
+      </c>
+      <c r="D90">
+        <v>-6.5</v>
+      </c>
+      <c r="E90">
+        <v>-6</v>
+      </c>
+      <c r="F90">
+        <v>-0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran mode jan 18
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BE31F3-40C5-49E5-BACC-25A04642F32F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303B6300-A4C9-44B0-BC74-4C90645A5A6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -542,11 +542,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="H86" sqref="H86"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2504,6 +2502,9 @@
       <c r="F85">
         <v>11</v>
       </c>
+      <c r="G85" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
@@ -2524,25 +2525,31 @@
       <c r="F86">
         <v>-20.8</v>
       </c>
+      <c r="G86" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>44213</v>
       </c>
       <c r="B87" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C87" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D87">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="E87">
-        <v>3.7</v>
+        <v>0.3</v>
       </c>
       <c r="F87">
-        <v>-1.2</v>
+        <v>0.7</v>
+      </c>
+      <c r="G87" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -2550,19 +2557,22 @@
         <v>44213</v>
       </c>
       <c r="B88" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C88" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D88">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E88">
-        <v>0.3</v>
+        <v>-10.7</v>
       </c>
       <c r="F88">
-        <v>0.7</v>
+        <v>13.2</v>
+      </c>
+      <c r="G88" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -2570,39 +2580,162 @@
         <v>44213</v>
       </c>
       <c r="B89" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C89" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D89">
-        <v>2.5</v>
+        <v>-6.5</v>
       </c>
       <c r="E89">
-        <v>-10.7</v>
+        <v>-6</v>
       </c>
       <c r="F89">
-        <v>13.2</v>
+        <v>-0.5</v>
+      </c>
+      <c r="G89" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
-        <v>44213</v>
+        <v>44214</v>
       </c>
       <c r="B90" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C90" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="D90">
+        <v>2</v>
+      </c>
+      <c r="E90">
+        <v>-6.3</v>
+      </c>
+      <c r="F90">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" s="2">
+        <v>44214</v>
+      </c>
+      <c r="B91" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" t="s">
+        <v>20</v>
+      </c>
+      <c r="D91">
+        <v>5.5</v>
+      </c>
+      <c r="E91">
+        <v>4</v>
+      </c>
+      <c r="F91">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="2">
+        <v>44214</v>
+      </c>
+      <c r="B92" t="s">
+        <v>35</v>
+      </c>
+      <c r="C92" t="s">
+        <v>30</v>
+      </c>
+      <c r="D92">
+        <v>-5</v>
+      </c>
+      <c r="E92">
+        <v>-7.2</v>
+      </c>
+      <c r="F92">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A93" s="2">
+        <v>44214</v>
+      </c>
+      <c r="B93" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s">
+        <v>19</v>
+      </c>
+      <c r="D93">
+        <v>3</v>
+      </c>
+      <c r="E93">
+        <v>-7.8</v>
+      </c>
+      <c r="F93">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A94" s="2">
+        <v>44214</v>
+      </c>
+      <c r="B94" t="s">
+        <v>15</v>
+      </c>
+      <c r="C94" t="s">
+        <v>24</v>
+      </c>
+      <c r="D94">
         <v>-6.5</v>
       </c>
-      <c r="E90">
-        <v>-6</v>
-      </c>
-      <c r="F90">
-        <v>-0.5</v>
+      <c r="E94">
+        <v>-16.3</v>
+      </c>
+      <c r="F94">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95" s="2">
+        <v>44214</v>
+      </c>
+      <c r="B95" t="s">
+        <v>36</v>
+      </c>
+      <c r="C95" t="s">
+        <v>26</v>
+      </c>
+      <c r="D95">
+        <v>2</v>
+      </c>
+      <c r="E95">
+        <v>-14.3</v>
+      </c>
+      <c r="F95">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A96" s="2">
+        <v>44214</v>
+      </c>
+      <c r="B96" t="s">
+        <v>23</v>
+      </c>
+      <c r="C96" t="s">
+        <v>22</v>
+      </c>
+      <c r="D96">
+        <v>-8.5</v>
+      </c>
+      <c r="E96">
+        <v>-10.199999999999999</v>
+      </c>
+      <c r="F96">
+        <v>1.6999999999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran model for 1/19/2021
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -1,26 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Documents\NBAPredictiveModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303B6300-A4C9-44B0-BC74-4C90645A5A6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7357737-6C5B-49B2-A2B2-6951D60F1EB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -542,9 +552,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2617,6 +2629,9 @@
       <c r="F90">
         <v>8.3000000000000007</v>
       </c>
+      <c r="G90" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
@@ -2637,6 +2652,9 @@
       <c r="F91">
         <v>1.5</v>
       </c>
+      <c r="G91" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
@@ -2657,6 +2675,9 @@
       <c r="F92">
         <v>2.2000000000000002</v>
       </c>
+      <c r="G92" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
@@ -2677,6 +2698,9 @@
       <c r="F93">
         <v>10.8</v>
       </c>
+      <c r="G93" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
@@ -2697,6 +2721,9 @@
       <c r="F94">
         <v>9.8000000000000007</v>
       </c>
+      <c r="G94" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
@@ -2717,6 +2744,9 @@
       <c r="F95">
         <v>16.3</v>
       </c>
+      <c r="G95" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
@@ -2736,6 +2766,49 @@
       </c>
       <c r="F96">
         <v>1.6999999999999991</v>
+      </c>
+      <c r="G96" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B97" t="s">
+        <v>9</v>
+      </c>
+      <c r="C97" t="s">
+        <v>32</v>
+      </c>
+      <c r="D97">
+        <v>-9.5</v>
+      </c>
+      <c r="E97">
+        <v>-1.6</v>
+      </c>
+      <c r="F97">
+        <v>-7.9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B98" t="s">
+        <v>34</v>
+      </c>
+      <c r="C98" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98">
+        <v>-6</v>
+      </c>
+      <c r="E98">
+        <v>-5.6</v>
+      </c>
+      <c r="F98">
+        <v>-0.40000000000000041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added games for 1/20/2021
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -1,36 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7357737-6C5B-49B2-A2B2-6951D60F1EB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA3057C-1F05-42B9-BC7D-07880D3A57B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -552,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="J107" sqref="J107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2771,7 +2761,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>44215</v>
       </c>
@@ -2790,8 +2780,11 @@
       <c r="F97">
         <v>-7.9</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G97" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>44215</v>
       </c>
@@ -2809,6 +2802,189 @@
       </c>
       <c r="F98">
         <v>-0.40000000000000041</v>
+      </c>
+      <c r="G98" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A99" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B99" t="s">
+        <v>31</v>
+      </c>
+      <c r="C99" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99">
+        <v>10</v>
+      </c>
+      <c r="E99">
+        <v>30.4</v>
+      </c>
+      <c r="F99">
+        <v>-20.399999999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A100" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B100" t="s">
+        <v>13</v>
+      </c>
+      <c r="C100" t="s">
+        <v>25</v>
+      </c>
+      <c r="D100">
+        <v>-5</v>
+      </c>
+      <c r="E100">
+        <v>-5.6</v>
+      </c>
+      <c r="F100">
+        <v>0.59999999999999964</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A101" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B101" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101" t="s">
+        <v>30</v>
+      </c>
+      <c r="D101">
+        <v>1.5</v>
+      </c>
+      <c r="E101">
+        <v>-6.7</v>
+      </c>
+      <c r="F101">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A102" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B102" t="s">
+        <v>16</v>
+      </c>
+      <c r="C102" t="s">
+        <v>24</v>
+      </c>
+      <c r="D102">
+        <v>-5</v>
+      </c>
+      <c r="E102">
+        <v>-2.5</v>
+      </c>
+      <c r="F102">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A103" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B103" t="s">
+        <v>35</v>
+      </c>
+      <c r="C103" t="s">
+        <v>15</v>
+      </c>
+      <c r="D103">
+        <v>-4.5</v>
+      </c>
+      <c r="E103">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F103">
+        <v>-13.3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A104" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B104" t="s">
+        <v>29</v>
+      </c>
+      <c r="C104" t="s">
+        <v>14</v>
+      </c>
+      <c r="D104">
+        <v>4</v>
+      </c>
+      <c r="E104">
+        <v>-5.3</v>
+      </c>
+      <c r="F104">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A105" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B105" t="s">
+        <v>26</v>
+      </c>
+      <c r="C105" t="s">
+        <v>20</v>
+      </c>
+      <c r="D105">
+        <v>5.5</v>
+      </c>
+      <c r="E105">
+        <v>-0.2</v>
+      </c>
+      <c r="F105">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A106" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B106" t="s">
+        <v>10</v>
+      </c>
+      <c r="C106" t="s">
+        <v>21</v>
+      </c>
+      <c r="D106">
+        <v>-9.5</v>
+      </c>
+      <c r="E106">
+        <v>-4</v>
+      </c>
+      <c r="F106">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A107" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B107" t="s">
+        <v>22</v>
+      </c>
+      <c r="C107" t="s">
+        <v>33</v>
+      </c>
+      <c r="D107">
+        <v>-1</v>
+      </c>
+      <c r="E107">
+        <v>-4.2</v>
+      </c>
+      <c r="F107">
+        <v>3.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added games for 1/21/2021
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA3057C-1F05-42B9-BC7D-07880D3A57B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C8E8E1-B57E-4732-B754-A8E5B518865D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="J107" sqref="J107"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="O97" sqref="O97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2826,6 +2826,9 @@
       <c r="F99">
         <v>-20.399999999999999</v>
       </c>
+      <c r="G99" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
@@ -2846,6 +2849,9 @@
       <c r="F100">
         <v>0.59999999999999964</v>
       </c>
+      <c r="G100" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
@@ -2866,6 +2872,9 @@
       <c r="F101">
         <v>8.1999999999999993</v>
       </c>
+      <c r="G101" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
@@ -2886,6 +2895,9 @@
       <c r="F102">
         <v>-2.5</v>
       </c>
+      <c r="G102" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
@@ -2906,6 +2918,9 @@
       <c r="F103">
         <v>-13.3</v>
       </c>
+      <c r="G103" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
@@ -2926,6 +2941,9 @@
       <c r="F104">
         <v>9.3000000000000007</v>
       </c>
+      <c r="G104" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
@@ -2946,6 +2964,9 @@
       <c r="F105">
         <v>5.7</v>
       </c>
+      <c r="G105" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
@@ -2966,6 +2987,9 @@
       <c r="F106">
         <v>-5.5</v>
       </c>
+      <c r="G106" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
@@ -2985,6 +3009,69 @@
       </c>
       <c r="F107">
         <v>3.2</v>
+      </c>
+      <c r="G107" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A108" s="2">
+        <v>44217</v>
+      </c>
+      <c r="B108" t="s">
+        <v>19</v>
+      </c>
+      <c r="C108" t="s">
+        <v>23</v>
+      </c>
+      <c r="D108">
+        <v>-1</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A109" s="2">
+        <v>44217</v>
+      </c>
+      <c r="B109" t="s">
+        <v>18</v>
+      </c>
+      <c r="C109" t="s">
+        <v>34</v>
+      </c>
+      <c r="D109">
+        <v>-7</v>
+      </c>
+      <c r="E109">
+        <v>7.5</v>
+      </c>
+      <c r="F109">
+        <v>-14.5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A110" s="2">
+        <v>44217</v>
+      </c>
+      <c r="B110" t="s">
+        <v>17</v>
+      </c>
+      <c r="C110" t="s">
+        <v>22</v>
+      </c>
+      <c r="D110">
+        <v>-4.5</v>
+      </c>
+      <c r="E110">
+        <v>11</v>
+      </c>
+      <c r="F110">
+        <v>-15.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran model for jan 23
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C8E8E1-B57E-4732-B754-A8E5B518865D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -142,11 +136,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,14 +204,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -264,7 +250,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -296,27 +282,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -348,24 +316,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -541,19 +491,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G110"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="O97" sqref="O97"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,7 +521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>44201</v>
       </c>
@@ -599,7 +544,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>44201</v>
       </c>
@@ -622,7 +567,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>44201</v>
       </c>
@@ -645,7 +590,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>44201</v>
       </c>
@@ -659,7 +604,7 @@
         <v>-9.5</v>
       </c>
       <c r="E5">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="F5">
         <v>-11.8</v>
@@ -668,7 +613,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>44201</v>
       </c>
@@ -685,13 +630,13 @@
         <v>7.4</v>
       </c>
       <c r="F6">
-        <v>-16.899999999999999</v>
+        <v>-16.9</v>
       </c>
       <c r="G6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>44202</v>
       </c>
@@ -714,7 +659,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>44202</v>
       </c>
@@ -737,7 +682,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>44202</v>
       </c>
@@ -754,13 +699,13 @@
         <v>-6.2</v>
       </c>
       <c r="F9">
-        <v>0.20000000000000021</v>
+        <v>0.2000000000000002</v>
       </c>
       <c r="G9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>44202</v>
       </c>
@@ -783,7 +728,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>44202</v>
       </c>
@@ -806,7 +751,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>44202</v>
       </c>
@@ -829,7 +774,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>44202</v>
       </c>
@@ -852,7 +797,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14" s="2">
         <v>44202</v>
       </c>
@@ -875,7 +820,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
         <v>44202</v>
       </c>
@@ -898,7 +843,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" s="2">
         <v>44202</v>
       </c>
@@ -921,7 +866,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
         <v>44202</v>
       </c>
@@ -944,7 +889,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18" s="2">
         <v>44203</v>
       </c>
@@ -967,7 +912,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
         <v>44203</v>
       </c>
@@ -990,7 +935,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20" s="2">
         <v>44203</v>
       </c>
@@ -1004,7 +949,7 @@
         <v>-10</v>
       </c>
       <c r="E20">
-        <v>-4.4000000000000004</v>
+        <v>-4.4</v>
       </c>
       <c r="F20">
         <v>-5.6</v>
@@ -1013,7 +958,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
         <v>44203</v>
       </c>
@@ -1036,7 +981,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22" s="2">
         <v>44203</v>
       </c>
@@ -1053,13 +998,13 @@
         <v>-6.2</v>
       </c>
       <c r="F22">
-        <v>-0.79999999999999982</v>
+        <v>-0.7999999999999998</v>
       </c>
       <c r="G22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23" s="2">
         <v>44204</v>
       </c>
@@ -1082,7 +1027,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24" s="2">
         <v>44204</v>
       </c>
@@ -1105,7 +1050,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25" s="2">
         <v>44204</v>
       </c>
@@ -1128,7 +1073,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26" s="2">
         <v>44204</v>
       </c>
@@ -1151,7 +1096,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="A27" s="2">
         <v>44204</v>
       </c>
@@ -1174,7 +1119,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28" s="2">
         <v>44204</v>
       </c>
@@ -1197,7 +1142,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="A29" s="2">
         <v>44204</v>
       </c>
@@ -1220,7 +1165,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30" s="2">
         <v>44204</v>
       </c>
@@ -1243,7 +1188,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7">
       <c r="A31" s="2">
         <v>44204</v>
       </c>
@@ -1266,7 +1211,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7">
       <c r="A32" s="2">
         <v>44204</v>
       </c>
@@ -1289,7 +1234,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7">
       <c r="A33" s="2">
         <v>44205</v>
       </c>
@@ -1312,7 +1257,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7">
       <c r="A34" s="2">
         <v>44205</v>
       </c>
@@ -1335,7 +1280,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7">
       <c r="A35" s="2">
         <v>44205</v>
       </c>
@@ -1352,13 +1297,13 @@
         <v>2.8</v>
       </c>
       <c r="F35">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="G35" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7">
       <c r="A36" s="2">
         <v>44205</v>
       </c>
@@ -1375,13 +1320,13 @@
         <v>-2.8</v>
       </c>
       <c r="F36">
-        <v>-0.20000000000000021</v>
+        <v>-0.2000000000000002</v>
       </c>
       <c r="G36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7">
       <c r="A37" s="2">
         <v>44205</v>
       </c>
@@ -1398,13 +1343,13 @@
         <v>3.7</v>
       </c>
       <c r="F37">
-        <v>0.79999999999999982</v>
+        <v>0.7999999999999998</v>
       </c>
       <c r="G37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7">
       <c r="A38" s="2">
         <v>44205</v>
       </c>
@@ -1421,13 +1366,13 @@
         <v>-26.9</v>
       </c>
       <c r="F38">
-        <v>16.399999999999999</v>
+        <v>16.4</v>
       </c>
       <c r="G38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7">
       <c r="A39" s="2">
         <v>44205</v>
       </c>
@@ -1450,7 +1395,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7">
       <c r="A40" s="2">
         <v>44205</v>
       </c>
@@ -1467,13 +1412,13 @@
         <v>0.1</v>
       </c>
       <c r="F40">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="G40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7">
       <c r="A41" s="2">
         <v>44206</v>
       </c>
@@ -1496,7 +1441,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7">
       <c r="A42" s="2">
         <v>44206</v>
       </c>
@@ -1519,7 +1464,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7">
       <c r="A43" s="2">
         <v>44206</v>
       </c>
@@ -1536,13 +1481,13 @@
         <v>11.7</v>
       </c>
       <c r="F43">
-        <v>-5.6999999999999993</v>
+        <v>-5.699999999999999</v>
       </c>
       <c r="G43" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7">
       <c r="A44" s="2">
         <v>44206</v>
       </c>
@@ -1559,13 +1504,13 @@
         <v>-13.6</v>
       </c>
       <c r="F44">
-        <v>5.0999999999999996</v>
+        <v>5.1</v>
       </c>
       <c r="G44" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7">
       <c r="A45" s="2">
         <v>44206</v>
       </c>
@@ -1579,16 +1524,16 @@
         <v>3.5</v>
       </c>
       <c r="E45">
-        <v>-1.1000000000000001</v>
+        <v>-1.1</v>
       </c>
       <c r="F45">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="G45" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7">
       <c r="A46" s="2">
         <v>44206</v>
       </c>
@@ -1611,7 +1556,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7">
       <c r="A47" s="2">
         <v>44206</v>
       </c>
@@ -1628,13 +1573,13 @@
         <v>-6.3</v>
       </c>
       <c r="F47">
-        <v>9.3000000000000007</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="G47" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7">
       <c r="A48" s="2">
         <v>44207</v>
       </c>
@@ -1657,7 +1602,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7">
       <c r="A49" s="2">
         <v>44207</v>
       </c>
@@ -1674,13 +1619,13 @@
         <v>-3.3</v>
       </c>
       <c r="F49">
-        <v>8.8000000000000007</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="G49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7">
       <c r="A50" s="2">
         <v>44207</v>
       </c>
@@ -1703,7 +1648,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7">
       <c r="A51" s="2">
         <v>44207</v>
       </c>
@@ -1726,7 +1671,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7">
       <c r="A52" s="2">
         <v>44207</v>
       </c>
@@ -1749,7 +1694,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7">
       <c r="A53" s="2">
         <v>44207</v>
       </c>
@@ -1766,13 +1711,13 @@
         <v>-2.8</v>
       </c>
       <c r="F53">
-        <v>-2.2000000000000002</v>
+        <v>-2.2</v>
       </c>
       <c r="G53" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7">
       <c r="A54" s="2">
         <v>44208</v>
       </c>
@@ -1795,7 +1740,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7">
       <c r="A55" s="2">
         <v>44208</v>
       </c>
@@ -1809,16 +1754,16 @@
         <v>-1</v>
       </c>
       <c r="E55">
-        <v>-8.1999999999999993</v>
+        <v>-8.199999999999999</v>
       </c>
       <c r="F55">
-        <v>7.1999999999999993</v>
+        <v>7.199999999999999</v>
       </c>
       <c r="G55" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7">
       <c r="A56" s="2">
         <v>44208</v>
       </c>
@@ -1841,7 +1786,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7">
       <c r="A57" s="2">
         <v>44208</v>
       </c>
@@ -1864,7 +1809,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7">
       <c r="A58" s="2">
         <v>44208</v>
       </c>
@@ -1878,16 +1823,16 @@
         <v>4.5</v>
       </c>
       <c r="E58">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="F58">
-        <v>0.40000000000000041</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="G58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7">
       <c r="A59" s="2">
         <v>44208</v>
       </c>
@@ -1904,13 +1849,13 @@
         <v>-2.8</v>
       </c>
       <c r="F59">
-        <v>-0.20000000000000021</v>
+        <v>-0.2000000000000002</v>
       </c>
       <c r="G59" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7">
       <c r="A60" s="2">
         <v>44209</v>
       </c>
@@ -1933,7 +1878,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7">
       <c r="A61" s="2">
         <v>44209</v>
       </c>
@@ -1956,7 +1901,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7">
       <c r="A62" s="2">
         <v>44209</v>
       </c>
@@ -1979,7 +1924,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7">
       <c r="A63" s="2">
         <v>44209</v>
       </c>
@@ -1993,7 +1938,7 @@
         <v>-3.5</v>
       </c>
       <c r="E63">
-        <v>-2.2999999999999998</v>
+        <v>-2.3</v>
       </c>
       <c r="F63">
         <v>-1.2</v>
@@ -2002,7 +1947,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7">
       <c r="A64" s="2">
         <v>44209</v>
       </c>
@@ -2019,13 +1964,13 @@
         <v>8.1</v>
       </c>
       <c r="F64">
-        <v>0.90000000000000036</v>
+        <v>0.9000000000000004</v>
       </c>
       <c r="G64" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7">
       <c r="A65" s="2">
         <v>44209</v>
       </c>
@@ -2048,7 +1993,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7">
       <c r="A66" s="2">
         <v>44209</v>
       </c>
@@ -2071,7 +2016,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7">
       <c r="A67" s="2">
         <v>44210</v>
       </c>
@@ -2094,7 +2039,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7">
       <c r="A68" s="2">
         <v>44210</v>
       </c>
@@ -2117,7 +2062,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7">
       <c r="A69" s="2">
         <v>44210</v>
       </c>
@@ -2140,7 +2085,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7">
       <c r="A70" s="2">
         <v>44210</v>
       </c>
@@ -2157,13 +2102,13 @@
         <v>-3.4</v>
       </c>
       <c r="F70">
-        <v>-1.1000000000000001</v>
+        <v>-1.1</v>
       </c>
       <c r="G70" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7">
       <c r="A71" s="2">
         <v>44210</v>
       </c>
@@ -2180,13 +2125,13 @@
         <v>-3.3</v>
       </c>
       <c r="F71">
-        <v>0.29999999999999982</v>
+        <v>0.2999999999999998</v>
       </c>
       <c r="G71" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7">
       <c r="A72" s="2">
         <v>44211</v>
       </c>
@@ -2209,7 +2154,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7">
       <c r="A73" s="2">
         <v>44211</v>
       </c>
@@ -2232,7 +2177,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7">
       <c r="A74" s="2">
         <v>44211</v>
       </c>
@@ -2255,7 +2200,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7">
       <c r="A75" s="2">
         <v>44211</v>
       </c>
@@ -2278,7 +2223,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7">
       <c r="A76" s="2">
         <v>44211</v>
       </c>
@@ -2301,7 +2246,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7">
       <c r="A77" s="2">
         <v>44211</v>
       </c>
@@ -2318,13 +2263,13 @@
         <v>-12.7</v>
       </c>
       <c r="F77">
-        <v>2.6999999999999988</v>
+        <v>2.699999999999999</v>
       </c>
       <c r="G77" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7">
       <c r="A78" s="2">
         <v>44211</v>
       </c>
@@ -2347,7 +2292,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7">
       <c r="A79" s="2">
         <v>44212</v>
       </c>
@@ -2370,7 +2315,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7">
       <c r="A80" s="2">
         <v>44212</v>
       </c>
@@ -2393,7 +2338,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7">
       <c r="A81" s="2">
         <v>44212</v>
       </c>
@@ -2416,7 +2361,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7">
       <c r="A82" s="2">
         <v>44212</v>
       </c>
@@ -2430,16 +2375,16 @@
         <v>-1.5</v>
       </c>
       <c r="E82">
-        <v>8.1999999999999993</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="F82">
-        <v>-9.6999999999999993</v>
+        <v>-9.699999999999999</v>
       </c>
       <c r="G82" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7">
       <c r="A83" s="2">
         <v>44212</v>
       </c>
@@ -2453,7 +2398,7 @@
         <v>-5</v>
       </c>
       <c r="E83">
-        <v>-18.600000000000001</v>
+        <v>-18.6</v>
       </c>
       <c r="F83">
         <v>13.6</v>
@@ -2462,7 +2407,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7">
       <c r="A84" s="2">
         <v>44212</v>
       </c>
@@ -2485,7 +2430,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7">
       <c r="A85" s="2">
         <v>44213</v>
       </c>
@@ -2508,7 +2453,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7">
       <c r="A86" s="2">
         <v>44213</v>
       </c>
@@ -2531,7 +2476,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7">
       <c r="A87" s="2">
         <v>44213</v>
       </c>
@@ -2554,7 +2499,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7">
       <c r="A88" s="2">
         <v>44213</v>
       </c>
@@ -2577,7 +2522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7">
       <c r="A89" s="2">
         <v>44213</v>
       </c>
@@ -2600,7 +2545,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7">
       <c r="A90" s="2">
         <v>44214</v>
       </c>
@@ -2617,13 +2562,13 @@
         <v>-6.3</v>
       </c>
       <c r="F90">
-        <v>8.3000000000000007</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="G90" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7">
       <c r="A91" s="2">
         <v>44214</v>
       </c>
@@ -2646,7 +2591,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7">
       <c r="A92" s="2">
         <v>44214</v>
       </c>
@@ -2663,13 +2608,13 @@
         <v>-7.2</v>
       </c>
       <c r="F92">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="G92" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7">
       <c r="A93" s="2">
         <v>44214</v>
       </c>
@@ -2692,7 +2637,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7">
       <c r="A94" s="2">
         <v>44214</v>
       </c>
@@ -2709,13 +2654,13 @@
         <v>-16.3</v>
       </c>
       <c r="F94">
-        <v>9.8000000000000007</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="G94" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7">
       <c r="A95" s="2">
         <v>44214</v>
       </c>
@@ -2738,7 +2683,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7">
       <c r="A96" s="2">
         <v>44214</v>
       </c>
@@ -2752,16 +2697,16 @@
         <v>-8.5</v>
       </c>
       <c r="E96">
-        <v>-10.199999999999999</v>
+        <v>-10.2</v>
       </c>
       <c r="F96">
-        <v>1.6999999999999991</v>
+        <v>1.699999999999999</v>
       </c>
       <c r="G96" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7">
       <c r="A97" s="2">
         <v>44215</v>
       </c>
@@ -2784,7 +2729,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7">
       <c r="A98" s="2">
         <v>44215</v>
       </c>
@@ -2801,13 +2746,13 @@
         <v>-5.6</v>
       </c>
       <c r="F98">
-        <v>-0.40000000000000041</v>
+        <v>-0.4000000000000004</v>
       </c>
       <c r="G98" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7">
       <c r="A99" s="2">
         <v>44216</v>
       </c>
@@ -2824,13 +2769,13 @@
         <v>30.4</v>
       </c>
       <c r="F99">
-        <v>-20.399999999999999</v>
+        <v>-20.4</v>
       </c>
       <c r="G99" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7">
       <c r="A100" s="2">
         <v>44216</v>
       </c>
@@ -2847,13 +2792,13 @@
         <v>-5.6</v>
       </c>
       <c r="F100">
-        <v>0.59999999999999964</v>
+        <v>0.5999999999999996</v>
       </c>
       <c r="G100" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7">
       <c r="A101" s="2">
         <v>44216</v>
       </c>
@@ -2870,13 +2815,13 @@
         <v>-6.7</v>
       </c>
       <c r="F101">
-        <v>8.1999999999999993</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="G101" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7">
       <c r="A102" s="2">
         <v>44216</v>
       </c>
@@ -2899,7 +2844,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7">
       <c r="A103" s="2">
         <v>44216</v>
       </c>
@@ -2913,7 +2858,7 @@
         <v>-4.5</v>
       </c>
       <c r="E103">
-        <v>8.8000000000000007</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="F103">
         <v>-13.3</v>
@@ -2922,7 +2867,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7">
       <c r="A104" s="2">
         <v>44216</v>
       </c>
@@ -2939,13 +2884,13 @@
         <v>-5.3</v>
       </c>
       <c r="F104">
-        <v>9.3000000000000007</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="G104" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7">
       <c r="A105" s="2">
         <v>44216</v>
       </c>
@@ -2968,7 +2913,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7">
       <c r="A106" s="2">
         <v>44216</v>
       </c>
@@ -2991,7 +2936,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7">
       <c r="A107" s="2">
         <v>44216</v>
       </c>
@@ -3014,7 +2959,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7">
       <c r="A108" s="2">
         <v>44217</v>
       </c>
@@ -3033,8 +2978,11 @@
       <c r="F108">
         <v>-1</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G108" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109" s="2">
         <v>44217</v>
       </c>
@@ -3053,8 +3001,11 @@
       <c r="F109">
         <v>-14.5</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G109" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
       <c r="A110" s="2">
         <v>44217</v>
       </c>
@@ -3072,6 +3023,149 @@
       </c>
       <c r="F110">
         <v>-15.5</v>
+      </c>
+      <c r="G110" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" s="2">
+        <v>44219</v>
+      </c>
+      <c r="B111" t="s">
+        <v>24</v>
+      </c>
+      <c r="C111" t="s">
+        <v>13</v>
+      </c>
+      <c r="D111">
+        <v>6.5</v>
+      </c>
+      <c r="E111">
+        <v>15.4</v>
+      </c>
+      <c r="F111">
+        <v>-8.9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" s="2">
+        <v>44219</v>
+      </c>
+      <c r="B112" t="s">
+        <v>7</v>
+      </c>
+      <c r="C112" t="s">
+        <v>15</v>
+      </c>
+      <c r="D112">
+        <v>-8</v>
+      </c>
+      <c r="E112">
+        <v>-5.8</v>
+      </c>
+      <c r="F112">
+        <v>-2.2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="2">
+        <v>44219</v>
+      </c>
+      <c r="B113" t="s">
+        <v>29</v>
+      </c>
+      <c r="C113" t="s">
+        <v>18</v>
+      </c>
+      <c r="D113">
+        <v>9.5</v>
+      </c>
+      <c r="E113">
+        <v>7</v>
+      </c>
+      <c r="F113">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" s="2">
+        <v>44219</v>
+      </c>
+      <c r="B114" t="s">
+        <v>34</v>
+      </c>
+      <c r="C114" t="s">
+        <v>22</v>
+      </c>
+      <c r="D114">
+        <v>-7</v>
+      </c>
+      <c r="E114">
+        <v>-11.7</v>
+      </c>
+      <c r="F114">
+        <v>4.699999999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="2">
+        <v>44219</v>
+      </c>
+      <c r="B115" t="s">
+        <v>36</v>
+      </c>
+      <c r="C115" t="s">
+        <v>23</v>
+      </c>
+      <c r="D115">
+        <v>9.5</v>
+      </c>
+      <c r="E115">
+        <v>-6</v>
+      </c>
+      <c r="F115">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" s="2">
+        <v>44219</v>
+      </c>
+      <c r="B116" t="s">
+        <v>30</v>
+      </c>
+      <c r="C116" t="s">
+        <v>26</v>
+      </c>
+      <c r="D116">
+        <v>-9.5</v>
+      </c>
+      <c r="E116">
+        <v>3.6</v>
+      </c>
+      <c r="F116">
+        <v>-13.1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="2">
+        <v>44219</v>
+      </c>
+      <c r="B117" t="s">
+        <v>20</v>
+      </c>
+      <c r="C117" t="s">
+        <v>9</v>
+      </c>
+      <c r="D117">
+        <v>1.5</v>
+      </c>
+      <c r="E117">
+        <v>-0.1</v>
+      </c>
+      <c r="F117">
+        <v>1.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran model for 1/24/2020
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854B355D-6EE6-417D-A900-77C6EC48EB29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -136,11 +142,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +210,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -250,7 +264,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -282,9 +296,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -316,6 +348,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -491,14 +541,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G117"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,7 +576,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44201</v>
       </c>
@@ -544,7 +599,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44201</v>
       </c>
@@ -567,7 +622,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44201</v>
       </c>
@@ -590,7 +645,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44201</v>
       </c>
@@ -604,7 +659,7 @@
         <v>-9.5</v>
       </c>
       <c r="E5">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F5">
         <v>-11.8</v>
@@ -613,7 +668,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44201</v>
       </c>
@@ -630,13 +685,13 @@
         <v>7.4</v>
       </c>
       <c r="F6">
-        <v>-16.9</v>
+        <v>-16.899999999999999</v>
       </c>
       <c r="G6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>44202</v>
       </c>
@@ -659,7 +714,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>44202</v>
       </c>
@@ -682,7 +737,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>44202</v>
       </c>
@@ -699,13 +754,13 @@
         <v>-6.2</v>
       </c>
       <c r="F9">
-        <v>0.2000000000000002</v>
+        <v>0.20000000000000021</v>
       </c>
       <c r="G9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>44202</v>
       </c>
@@ -728,7 +783,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44202</v>
       </c>
@@ -751,7 +806,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>44202</v>
       </c>
@@ -774,7 +829,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44202</v>
       </c>
@@ -797,7 +852,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>44202</v>
       </c>
@@ -820,7 +875,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>44202</v>
       </c>
@@ -843,7 +898,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>44202</v>
       </c>
@@ -866,7 +921,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44202</v>
       </c>
@@ -889,7 +944,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>44203</v>
       </c>
@@ -912,7 +967,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>44203</v>
       </c>
@@ -935,7 +990,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>44203</v>
       </c>
@@ -949,7 +1004,7 @@
         <v>-10</v>
       </c>
       <c r="E20">
-        <v>-4.4</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="F20">
         <v>-5.6</v>
@@ -958,7 +1013,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>44203</v>
       </c>
@@ -981,7 +1036,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>44203</v>
       </c>
@@ -998,13 +1053,13 @@
         <v>-6.2</v>
       </c>
       <c r="F22">
-        <v>-0.7999999999999998</v>
+        <v>-0.79999999999999982</v>
       </c>
       <c r="G22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>44204</v>
       </c>
@@ -1027,7 +1082,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>44204</v>
       </c>
@@ -1050,7 +1105,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>44204</v>
       </c>
@@ -1073,7 +1128,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>44204</v>
       </c>
@@ -1096,7 +1151,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>44204</v>
       </c>
@@ -1119,7 +1174,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>44204</v>
       </c>
@@ -1142,7 +1197,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>44204</v>
       </c>
@@ -1165,7 +1220,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>44204</v>
       </c>
@@ -1188,7 +1243,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>44204</v>
       </c>
@@ -1211,7 +1266,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>44204</v>
       </c>
@@ -1234,7 +1289,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>44205</v>
       </c>
@@ -1257,7 +1312,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>44205</v>
       </c>
@@ -1280,7 +1335,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>44205</v>
       </c>
@@ -1297,13 +1352,13 @@
         <v>2.8</v>
       </c>
       <c r="F35">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G35" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>44205</v>
       </c>
@@ -1320,13 +1375,13 @@
         <v>-2.8</v>
       </c>
       <c r="F36">
-        <v>-0.2000000000000002</v>
+        <v>-0.20000000000000021</v>
       </c>
       <c r="G36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>44205</v>
       </c>
@@ -1343,13 +1398,13 @@
         <v>3.7</v>
       </c>
       <c r="F37">
-        <v>0.7999999999999998</v>
+        <v>0.79999999999999982</v>
       </c>
       <c r="G37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>44205</v>
       </c>
@@ -1366,13 +1421,13 @@
         <v>-26.9</v>
       </c>
       <c r="F38">
-        <v>16.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="G38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>44205</v>
       </c>
@@ -1395,7 +1450,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>44205</v>
       </c>
@@ -1412,13 +1467,13 @@
         <v>0.1</v>
       </c>
       <c r="F40">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>44206</v>
       </c>
@@ -1441,7 +1496,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>44206</v>
       </c>
@@ -1464,7 +1519,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>44206</v>
       </c>
@@ -1481,13 +1536,13 @@
         <v>11.7</v>
       </c>
       <c r="F43">
-        <v>-5.699999999999999</v>
+        <v>-5.6999999999999993</v>
       </c>
       <c r="G43" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>44206</v>
       </c>
@@ -1504,13 +1559,13 @@
         <v>-13.6</v>
       </c>
       <c r="F44">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G44" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44206</v>
       </c>
@@ -1524,16 +1579,16 @@
         <v>3.5</v>
       </c>
       <c r="E45">
-        <v>-1.1</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="F45">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="G45" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>44206</v>
       </c>
@@ -1556,7 +1611,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>44206</v>
       </c>
@@ -1573,13 +1628,13 @@
         <v>-6.3</v>
       </c>
       <c r="F47">
-        <v>9.300000000000001</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="G47" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>44207</v>
       </c>
@@ -1602,7 +1657,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>44207</v>
       </c>
@@ -1619,13 +1674,13 @@
         <v>-3.3</v>
       </c>
       <c r="F49">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="G49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>44207</v>
       </c>
@@ -1648,7 +1703,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>44207</v>
       </c>
@@ -1671,7 +1726,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>44207</v>
       </c>
@@ -1694,7 +1749,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>44207</v>
       </c>
@@ -1711,13 +1766,13 @@
         <v>-2.8</v>
       </c>
       <c r="F53">
-        <v>-2.2</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="G53" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>44208</v>
       </c>
@@ -1740,7 +1795,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>44208</v>
       </c>
@@ -1754,16 +1809,16 @@
         <v>-1</v>
       </c>
       <c r="E55">
-        <v>-8.199999999999999</v>
+        <v>-8.1999999999999993</v>
       </c>
       <c r="F55">
-        <v>7.199999999999999</v>
+        <v>7.1999999999999993</v>
       </c>
       <c r="G55" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>44208</v>
       </c>
@@ -1786,7 +1841,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>44208</v>
       </c>
@@ -1809,7 +1864,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>44208</v>
       </c>
@@ -1823,16 +1878,16 @@
         <v>4.5</v>
       </c>
       <c r="E58">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F58">
-        <v>0.4000000000000004</v>
+        <v>0.40000000000000041</v>
       </c>
       <c r="G58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>44208</v>
       </c>
@@ -1849,13 +1904,13 @@
         <v>-2.8</v>
       </c>
       <c r="F59">
-        <v>-0.2000000000000002</v>
+        <v>-0.20000000000000021</v>
       </c>
       <c r="G59" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>44209</v>
       </c>
@@ -1878,7 +1933,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>44209</v>
       </c>
@@ -1901,7 +1956,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>44209</v>
       </c>
@@ -1924,7 +1979,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>44209</v>
       </c>
@@ -1938,7 +1993,7 @@
         <v>-3.5</v>
       </c>
       <c r="E63">
-        <v>-2.3</v>
+        <v>-2.2999999999999998</v>
       </c>
       <c r="F63">
         <v>-1.2</v>
@@ -1947,7 +2002,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>44209</v>
       </c>
@@ -1964,13 +2019,13 @@
         <v>8.1</v>
       </c>
       <c r="F64">
-        <v>0.9000000000000004</v>
+        <v>0.90000000000000036</v>
       </c>
       <c r="G64" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>44209</v>
       </c>
@@ -1993,7 +2048,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>44209</v>
       </c>
@@ -2016,7 +2071,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>44210</v>
       </c>
@@ -2039,7 +2094,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>44210</v>
       </c>
@@ -2062,7 +2117,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>44210</v>
       </c>
@@ -2085,7 +2140,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>44210</v>
       </c>
@@ -2102,13 +2157,13 @@
         <v>-3.4</v>
       </c>
       <c r="F70">
-        <v>-1.1</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="G70" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>44210</v>
       </c>
@@ -2125,13 +2180,13 @@
         <v>-3.3</v>
       </c>
       <c r="F71">
-        <v>0.2999999999999998</v>
+        <v>0.29999999999999982</v>
       </c>
       <c r="G71" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>44211</v>
       </c>
@@ -2154,7 +2209,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>44211</v>
       </c>
@@ -2177,7 +2232,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>44211</v>
       </c>
@@ -2200,7 +2255,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>44211</v>
       </c>
@@ -2223,7 +2278,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>44211</v>
       </c>
@@ -2246,7 +2301,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>44211</v>
       </c>
@@ -2263,13 +2318,13 @@
         <v>-12.7</v>
       </c>
       <c r="F77">
-        <v>2.699999999999999</v>
+        <v>2.6999999999999988</v>
       </c>
       <c r="G77" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>44211</v>
       </c>
@@ -2292,7 +2347,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>44212</v>
       </c>
@@ -2315,7 +2370,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>44212</v>
       </c>
@@ -2338,7 +2393,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>44212</v>
       </c>
@@ -2361,7 +2416,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>44212</v>
       </c>
@@ -2375,16 +2430,16 @@
         <v>-1.5</v>
       </c>
       <c r="E82">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="F82">
-        <v>-9.699999999999999</v>
+        <v>-9.6999999999999993</v>
       </c>
       <c r="G82" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>44212</v>
       </c>
@@ -2398,7 +2453,7 @@
         <v>-5</v>
       </c>
       <c r="E83">
-        <v>-18.6</v>
+        <v>-18.600000000000001</v>
       </c>
       <c r="F83">
         <v>13.6</v>
@@ -2407,7 +2462,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>44212</v>
       </c>
@@ -2430,7 +2485,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>44213</v>
       </c>
@@ -2453,7 +2508,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>44213</v>
       </c>
@@ -2476,7 +2531,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>44213</v>
       </c>
@@ -2499,7 +2554,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>44213</v>
       </c>
@@ -2522,7 +2577,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>44213</v>
       </c>
@@ -2545,7 +2600,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>44214</v>
       </c>
@@ -2562,13 +2617,13 @@
         <v>-6.3</v>
       </c>
       <c r="F90">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="G90" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>44214</v>
       </c>
@@ -2591,7 +2646,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>44214</v>
       </c>
@@ -2608,13 +2663,13 @@
         <v>-7.2</v>
       </c>
       <c r="F92">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G92" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>44214</v>
       </c>
@@ -2637,7 +2692,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>44214</v>
       </c>
@@ -2654,13 +2709,13 @@
         <v>-16.3</v>
       </c>
       <c r="F94">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="G94" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>44214</v>
       </c>
@@ -2683,7 +2738,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>44214</v>
       </c>
@@ -2697,16 +2752,16 @@
         <v>-8.5</v>
       </c>
       <c r="E96">
-        <v>-10.2</v>
+        <v>-10.199999999999999</v>
       </c>
       <c r="F96">
-        <v>1.699999999999999</v>
+        <v>1.6999999999999991</v>
       </c>
       <c r="G96" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>44215</v>
       </c>
@@ -2729,7 +2784,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>44215</v>
       </c>
@@ -2746,13 +2801,13 @@
         <v>-5.6</v>
       </c>
       <c r="F98">
-        <v>-0.4000000000000004</v>
+        <v>-0.40000000000000041</v>
       </c>
       <c r="G98" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>44216</v>
       </c>
@@ -2769,13 +2824,13 @@
         <v>30.4</v>
       </c>
       <c r="F99">
-        <v>-20.4</v>
+        <v>-20.399999999999999</v>
       </c>
       <c r="G99" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>44216</v>
       </c>
@@ -2792,13 +2847,13 @@
         <v>-5.6</v>
       </c>
       <c r="F100">
-        <v>0.5999999999999996</v>
+        <v>0.59999999999999964</v>
       </c>
       <c r="G100" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>44216</v>
       </c>
@@ -2815,13 +2870,13 @@
         <v>-6.7</v>
       </c>
       <c r="F101">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="G101" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>44216</v>
       </c>
@@ -2844,7 +2899,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>44216</v>
       </c>
@@ -2858,7 +2913,7 @@
         <v>-4.5</v>
       </c>
       <c r="E103">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="F103">
         <v>-13.3</v>
@@ -2867,7 +2922,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>44216</v>
       </c>
@@ -2884,13 +2939,13 @@
         <v>-5.3</v>
       </c>
       <c r="F104">
-        <v>9.300000000000001</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="G104" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>44216</v>
       </c>
@@ -2913,7 +2968,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>44216</v>
       </c>
@@ -2936,7 +2991,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>44216</v>
       </c>
@@ -2959,7 +3014,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>44217</v>
       </c>
@@ -2982,7 +3037,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>44217</v>
       </c>
@@ -3005,7 +3060,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>44217</v>
       </c>
@@ -3028,7 +3083,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>44219</v>
       </c>
@@ -3047,8 +3102,11 @@
       <c r="F111">
         <v>-8.9</v>
       </c>
-    </row>
-    <row r="112" spans="1:7">
+      <c r="G111" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>44219</v>
       </c>
@@ -3065,10 +3123,13 @@
         <v>-5.8</v>
       </c>
       <c r="F112">
-        <v>-2.2</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="G112" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>44219</v>
       </c>
@@ -3087,8 +3148,11 @@
       <c r="F113">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="114" spans="1:6">
+      <c r="G113" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>44219</v>
       </c>
@@ -3105,10 +3169,13 @@
         <v>-11.7</v>
       </c>
       <c r="F114">
-        <v>4.699999999999999</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
+        <v>4.6999999999999993</v>
+      </c>
+      <c r="G114" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>44219</v>
       </c>
@@ -3127,8 +3194,11 @@
       <c r="F115">
         <v>15.5</v>
       </c>
-    </row>
-    <row r="116" spans="1:6">
+      <c r="G115" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>44219</v>
       </c>
@@ -3147,8 +3217,11 @@
       <c r="F116">
         <v>-13.1</v>
       </c>
-    </row>
-    <row r="117" spans="1:6">
+      <c r="G116" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>44219</v>
       </c>
@@ -3166,6 +3239,149 @@
       </c>
       <c r="F117">
         <v>1.6</v>
+      </c>
+      <c r="G117" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A118" s="2">
+        <v>44220</v>
+      </c>
+      <c r="B118" t="s">
+        <v>12</v>
+      </c>
+      <c r="C118" t="s">
+        <v>35</v>
+      </c>
+      <c r="D118">
+        <v>-4.5</v>
+      </c>
+      <c r="E118">
+        <v>1.7</v>
+      </c>
+      <c r="F118">
+        <v>-6.2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A119" s="2">
+        <v>44220</v>
+      </c>
+      <c r="B119" t="s">
+        <v>10</v>
+      </c>
+      <c r="C119" t="s">
+        <v>32</v>
+      </c>
+      <c r="D119">
+        <v>-13</v>
+      </c>
+      <c r="E119">
+        <v>-14.5</v>
+      </c>
+      <c r="F119">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A120" s="2">
+        <v>44220</v>
+      </c>
+      <c r="B120" t="s">
+        <v>25</v>
+      </c>
+      <c r="C120" t="s">
+        <v>31</v>
+      </c>
+      <c r="D120">
+        <v>-6</v>
+      </c>
+      <c r="E120">
+        <v>-1.9</v>
+      </c>
+      <c r="F120">
+        <v>-4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A121" s="2">
+        <v>44220</v>
+      </c>
+      <c r="B121" t="s">
+        <v>14</v>
+      </c>
+      <c r="C121" t="s">
+        <v>28</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+      <c r="E121">
+        <v>7.9</v>
+      </c>
+      <c r="F121">
+        <v>-6.9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A122" s="2">
+        <v>44220</v>
+      </c>
+      <c r="B122" t="s">
+        <v>19</v>
+      </c>
+      <c r="C122" t="s">
+        <v>16</v>
+      </c>
+      <c r="D122">
+        <v>-8.5</v>
+      </c>
+      <c r="E122">
+        <v>-11.9</v>
+      </c>
+      <c r="F122">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A123" s="2">
+        <v>44220</v>
+      </c>
+      <c r="B123" t="s">
+        <v>33</v>
+      </c>
+      <c r="C123" t="s">
+        <v>27</v>
+      </c>
+      <c r="D123">
+        <v>-7.5</v>
+      </c>
+      <c r="E123">
+        <v>8.9</v>
+      </c>
+      <c r="F123">
+        <v>-16.399999999999999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A124" s="2">
+        <v>44220</v>
+      </c>
+      <c r="B124" t="s">
+        <v>11</v>
+      </c>
+      <c r="C124" t="s">
+        <v>17</v>
+      </c>
+      <c r="D124">
+        <v>-4</v>
+      </c>
+      <c r="E124">
+        <v>-11.1</v>
+      </c>
+      <c r="F124">
+        <v>7.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added games for 1/25/2021
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854B355D-6EE6-417D-A900-77C6EC48EB29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B15A44-D0A3-485C-A6DA-6B1160B5D2E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3263,6 +3263,9 @@
       <c r="F118">
         <v>-6.2</v>
       </c>
+      <c r="G118" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
@@ -3283,6 +3286,9 @@
       <c r="F119">
         <v>1.5</v>
       </c>
+      <c r="G119" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
@@ -3303,6 +3309,9 @@
       <c r="F120">
         <v>-4.0999999999999996</v>
       </c>
+      <c r="G120" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
@@ -3323,6 +3332,9 @@
       <c r="F121">
         <v>-6.9</v>
       </c>
+      <c r="G121" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
@@ -3343,6 +3355,9 @@
       <c r="F122">
         <v>3.4</v>
       </c>
+      <c r="G122" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
@@ -3363,6 +3378,9 @@
       <c r="F123">
         <v>-16.399999999999999</v>
       </c>
+      <c r="G123" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
@@ -3382,6 +3400,189 @@
       </c>
       <c r="F124">
         <v>7.1</v>
+      </c>
+      <c r="G124" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A125" s="2">
+        <v>44221</v>
+      </c>
+      <c r="B125" t="s">
+        <v>12</v>
+      </c>
+      <c r="C125" t="s">
+        <v>35</v>
+      </c>
+      <c r="D125">
+        <v>-2</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A126" s="2">
+        <v>44221</v>
+      </c>
+      <c r="B126" t="s">
+        <v>14</v>
+      </c>
+      <c r="C126" t="s">
+        <v>28</v>
+      </c>
+      <c r="D126">
+        <v>-1.5</v>
+      </c>
+      <c r="E126">
+        <v>5.4</v>
+      </c>
+      <c r="F126">
+        <v>-6.9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A127" s="2">
+        <v>44221</v>
+      </c>
+      <c r="B127" t="s">
+        <v>24</v>
+      </c>
+      <c r="C127" t="s">
+        <v>13</v>
+      </c>
+      <c r="D127">
+        <v>5</v>
+      </c>
+      <c r="E127">
+        <v>12.8</v>
+      </c>
+      <c r="F127">
+        <v>-7.8000000000000007</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A128" s="2">
+        <v>44221</v>
+      </c>
+      <c r="B128" t="s">
+        <v>7</v>
+      </c>
+      <c r="C128" t="s">
+        <v>15</v>
+      </c>
+      <c r="D128">
+        <v>-7.5</v>
+      </c>
+      <c r="E128">
+        <v>-7.2</v>
+      </c>
+      <c r="F128">
+        <v>-0.29999999999999982</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" s="2">
+        <v>44221</v>
+      </c>
+      <c r="B129" t="s">
+        <v>31</v>
+      </c>
+      <c r="C129" t="s">
+        <v>23</v>
+      </c>
+      <c r="D129">
+        <v>12</v>
+      </c>
+      <c r="E129">
+        <v>12.4</v>
+      </c>
+      <c r="F129">
+        <v>-0.40000000000000041</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" s="2">
+        <v>44221</v>
+      </c>
+      <c r="B130" t="s">
+        <v>30</v>
+      </c>
+      <c r="C130" t="s">
+        <v>9</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
+      </c>
+      <c r="E130">
+        <v>3.9</v>
+      </c>
+      <c r="F130">
+        <v>-1.9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131" s="2">
+        <v>44221</v>
+      </c>
+      <c r="B131" t="s">
+        <v>36</v>
+      </c>
+      <c r="C131" t="s">
+        <v>25</v>
+      </c>
+      <c r="D131">
+        <v>3.5</v>
+      </c>
+      <c r="E131">
+        <v>-8.5</v>
+      </c>
+      <c r="F131">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132" s="2">
+        <v>44221</v>
+      </c>
+      <c r="B132" t="s">
+        <v>22</v>
+      </c>
+      <c r="C132" t="s">
+        <v>29</v>
+      </c>
+      <c r="D132">
+        <v>-8.5</v>
+      </c>
+      <c r="E132">
+        <v>-6.3</v>
+      </c>
+      <c r="F132">
+        <v>-2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" s="2">
+        <v>44221</v>
+      </c>
+      <c r="B133" t="s">
+        <v>11</v>
+      </c>
+      <c r="C133" t="s">
+        <v>32</v>
+      </c>
+      <c r="D133">
+        <v>-5</v>
+      </c>
+      <c r="E133">
+        <v>-1.8</v>
+      </c>
+      <c r="F133">
+        <v>-3.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran model jan 26
</commit_message>
<xml_diff>
--- a/NBAGames.xlsx
+++ b/NBAGames.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\NBAPredictiveModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Documents\NBAPredictiveModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B15A44-D0A3-485C-A6DA-6B1160B5D2E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6083B908-A5CB-43AF-916F-6DC674F1C414}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -542,11 +542,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G133"/>
+  <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="E135" sqref="E135"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3424,6 +3422,9 @@
       <c r="F125">
         <v>-2</v>
       </c>
+      <c r="G125" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
@@ -3444,6 +3445,9 @@
       <c r="F126">
         <v>-6.9</v>
       </c>
+      <c r="G126" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
@@ -3464,6 +3468,9 @@
       <c r="F127">
         <v>-7.8000000000000007</v>
       </c>
+      <c r="G127" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
@@ -3484,8 +3491,11 @@
       <c r="F128">
         <v>-0.29999999999999982</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G128" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <v>44221</v>
       </c>
@@ -3504,8 +3514,11 @@
       <c r="F129">
         <v>-0.40000000000000041</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G129" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>44221</v>
       </c>
@@ -3524,8 +3537,11 @@
       <c r="F130">
         <v>-1.9</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G130" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
         <v>44221</v>
       </c>
@@ -3544,8 +3560,11 @@
       <c r="F131">
         <v>12</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G131" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <v>44221</v>
       </c>
@@ -3564,8 +3583,11 @@
       <c r="F132">
         <v>-2.2000000000000002</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G132" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
         <v>44221</v>
       </c>
@@ -3583,6 +3605,69 @@
       </c>
       <c r="F133">
         <v>-3.2</v>
+      </c>
+      <c r="G133" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A134" s="2">
+        <v>44222</v>
+      </c>
+      <c r="B134" t="s">
+        <v>16</v>
+      </c>
+      <c r="C134" t="s">
+        <v>10</v>
+      </c>
+      <c r="D134">
+        <v>-5</v>
+      </c>
+      <c r="E134">
+        <v>11</v>
+      </c>
+      <c r="F134">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A135" s="2">
+        <v>44222</v>
+      </c>
+      <c r="B135" t="s">
+        <v>26</v>
+      </c>
+      <c r="C135" t="s">
+        <v>27</v>
+      </c>
+      <c r="D135">
+        <v>-3.5</v>
+      </c>
+      <c r="E135">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F135">
+        <v>-8.1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136" s="2">
+        <v>44222</v>
+      </c>
+      <c r="B136" t="s">
+        <v>34</v>
+      </c>
+      <c r="C136" t="s">
+        <v>17</v>
+      </c>
+      <c r="D136">
+        <v>-11</v>
+      </c>
+      <c r="E136">
+        <v>-22.2</v>
+      </c>
+      <c r="F136">
+        <v>11.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>